<commit_message>
Add screenshots in README
</commit_message>
<xml_diff>
--- a/docs/tasks.xlsx
+++ b/docs/tasks.xlsx
@@ -1,16 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28730"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\dev\git\web\plan-it\doc\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4BC65C7-08E9-48C7-9B37-EA2648B6AD4F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15390" tabRatio="438" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20610" windowHeight="11640" tabRatio="438"/>
   </bookViews>
   <sheets>
     <sheet name="Requirements" sheetId="1" r:id="rId1"/>
@@ -23,7 +17,7 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Defects!$B$1:$E$34</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Requirements!$B$1:$F$69</definedName>
   </definedNames>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="125725"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -145,12 +139,12 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="2">
     <numFmt numFmtId="42" formatCode="_-&quot;₩&quot;* #,##0_-;\-&quot;₩&quot;* #,##0_-;_-&quot;₩&quot;* &quot;-&quot;_-;_-@_-"/>
     <numFmt numFmtId="176" formatCode="yy&quot;-&quot;m&quot;-&quot;d;@"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <name val="돋움"/>
@@ -280,7 +274,7 @@
         <xdr:cNvPr id="2" name="TextBox 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000002000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0400-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -326,9 +320,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 테마">
   <a:themeElements>
-    <a:clrScheme name="Office 2007 - 2010">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -366,7 +360,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office 2007 - 2010">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -400,7 +394,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -435,10 +428,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office 2007 - 2010">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -611,14 +603,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:F165"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5" customHeight="1" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultRowHeight="16.5" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="2.77734375" style="9" customWidth="1"/>
     <col min="2" max="2" width="59.21875" style="1" customWidth="1"/>
@@ -629,7 +621,7 @@
     <col min="7" max="16384" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="27" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:6" ht="27" customHeight="1">
       <c r="A1" s="7"/>
       <c r="B1" s="5" t="s">
         <v>0</v>
@@ -647,7 +639,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:6" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:6" customFormat="1" ht="16.5" customHeight="1">
       <c r="A2" s="3"/>
       <c r="B2" s="13" t="s">
         <v>12</v>
@@ -664,7 +656,7 @@
       </c>
       <c r="F2" s="12"/>
     </row>
-    <row r="3" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:6" ht="16.5" customHeight="1">
       <c r="A3" s="8"/>
       <c r="B3" s="13" t="s">
         <v>11</v>
@@ -677,7 +669,7 @@
         <v>45777</v>
       </c>
     </row>
-    <row r="4" spans="1:6" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:6" customFormat="1" ht="16.5" customHeight="1">
       <c r="A4" s="3"/>
       <c r="B4" t="s">
         <v>13</v>
@@ -696,7 +688,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:6" ht="16.5" customHeight="1">
       <c r="A5" s="8"/>
       <c r="B5" s="1" t="s">
         <v>14</v>
@@ -709,7 +701,7 @@
         <v>45777</v>
       </c>
     </row>
-    <row r="6" spans="1:6" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:6" customFormat="1" ht="16.5" customHeight="1">
       <c r="A6" s="3"/>
       <c r="B6" t="s">
         <v>17</v>
@@ -726,7 +718,7 @@
       </c>
       <c r="F6" s="12"/>
     </row>
-    <row r="7" spans="1:6" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:6" customFormat="1" ht="18" customHeight="1">
       <c r="A7" s="3"/>
       <c r="B7" t="s">
         <v>18</v>
@@ -743,7 +735,7 @@
       </c>
       <c r="F7" s="12"/>
     </row>
-    <row r="8" spans="1:6" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:6" customFormat="1" ht="17.25" customHeight="1">
       <c r="A8" s="3"/>
       <c r="B8" s="1" t="s">
         <v>19</v>
@@ -758,7 +750,7 @@
       <c r="E8" s="15"/>
       <c r="F8" s="12"/>
     </row>
-    <row r="9" spans="1:6" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:6" customFormat="1" ht="16.5" customHeight="1">
       <c r="A9" s="3"/>
       <c r="B9" t="s">
         <v>22</v>
@@ -775,29 +767,31 @@
       </c>
       <c r="F9" s="12"/>
     </row>
-    <row r="10" spans="1:6" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:6" customFormat="1" ht="16.5" customHeight="1">
       <c r="A10" s="3"/>
       <c r="B10" t="s">
         <v>23</v>
       </c>
       <c r="C10" s="3" t="str">
         <f t="shared" si="0"/>
-        <v/>
+        <v>✓</v>
       </c>
       <c r="D10" s="15">
         <v>45780</v>
       </c>
-      <c r="E10" s="15"/>
+      <c r="E10" s="15">
+        <v>45827</v>
+      </c>
       <c r="F10" s="12"/>
     </row>
-    <row r="11" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:6" ht="16.5" customHeight="1">
       <c r="A11" s="8"/>
       <c r="C11" s="3" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
-    <row r="12" spans="1:6" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:6" customFormat="1" ht="16.5" customHeight="1">
       <c r="A12" s="3"/>
       <c r="C12" s="3" t="str">
         <f t="shared" si="0"/>
@@ -807,7 +801,7 @@
       <c r="E12" s="15"/>
       <c r="F12" s="12"/>
     </row>
-    <row r="13" spans="1:6" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:6" customFormat="1" ht="20.25" customHeight="1">
       <c r="A13" s="3"/>
       <c r="C13" s="3" t="str">
         <f t="shared" si="0"/>
@@ -817,7 +811,7 @@
       <c r="E13" s="15"/>
       <c r="F13" s="12"/>
     </row>
-    <row r="14" spans="1:6" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:6" customFormat="1" ht="20.25" customHeight="1">
       <c r="A14" s="3"/>
       <c r="C14" s="3" t="str">
         <f t="shared" si="0"/>
@@ -827,7 +821,7 @@
       <c r="E14" s="15"/>
       <c r="F14" s="12"/>
     </row>
-    <row r="15" spans="1:6" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:6" customFormat="1" ht="16.5" customHeight="1">
       <c r="A15" s="3"/>
       <c r="C15" s="3" t="str">
         <f t="shared" si="0"/>
@@ -837,7 +831,7 @@
       <c r="E15" s="15"/>
       <c r="F15" s="12"/>
     </row>
-    <row r="16" spans="1:6" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:6" customFormat="1" ht="16.5" customHeight="1">
       <c r="A16" s="3"/>
       <c r="C16" s="3" t="str">
         <f t="shared" si="0"/>
@@ -847,14 +841,14 @@
       <c r="E16" s="15"/>
       <c r="F16" s="12"/>
     </row>
-    <row r="17" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:6" ht="16.5" customHeight="1">
       <c r="A17" s="8"/>
       <c r="C17" s="3" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
-    <row r="18" spans="1:6" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:6" customFormat="1" ht="16.5" customHeight="1">
       <c r="A18" s="3"/>
       <c r="C18" s="3" t="str">
         <f t="shared" si="0"/>
@@ -864,7 +858,7 @@
       <c r="E18" s="15"/>
       <c r="F18" s="12"/>
     </row>
-    <row r="19" spans="1:6" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:6" customFormat="1" ht="16.5" customHeight="1">
       <c r="A19" s="3"/>
       <c r="C19" s="3" t="str">
         <f t="shared" si="0"/>
@@ -874,7 +868,7 @@
       <c r="E19" s="15"/>
       <c r="F19" s="12"/>
     </row>
-    <row r="20" spans="1:6" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:6" customFormat="1" ht="16.5" customHeight="1">
       <c r="A20" s="3"/>
       <c r="C20" s="3" t="str">
         <f t="shared" si="0"/>
@@ -884,7 +878,7 @@
       <c r="E20" s="15"/>
       <c r="F20" s="12"/>
     </row>
-    <row r="21" spans="1:6" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:6" customFormat="1" ht="16.5" customHeight="1">
       <c r="A21" s="3"/>
       <c r="C21" s="3" t="str">
         <f t="shared" si="0"/>
@@ -894,7 +888,7 @@
       <c r="E21" s="15"/>
       <c r="F21" s="12"/>
     </row>
-    <row r="22" spans="1:6" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:6" customFormat="1" ht="16.5" customHeight="1">
       <c r="A22" s="3"/>
       <c r="C22" s="3" t="str">
         <f t="shared" si="0"/>
@@ -904,14 +898,14 @@
       <c r="E22" s="15"/>
       <c r="F22" s="12"/>
     </row>
-    <row r="23" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:6" ht="16.5" customHeight="1">
       <c r="A23" s="8"/>
       <c r="C23" s="3" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
-    <row r="24" spans="1:6" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="24" spans="1:6" customFormat="1" ht="16.5" customHeight="1">
       <c r="A24" s="3"/>
       <c r="C24" s="3" t="str">
         <f t="shared" si="0"/>
@@ -921,7 +915,7 @@
       <c r="E24" s="15"/>
       <c r="F24" s="12"/>
     </row>
-    <row r="25" spans="1:6" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="25" spans="1:6" customFormat="1" ht="16.5" customHeight="1">
       <c r="A25" s="3"/>
       <c r="C25" s="3" t="str">
         <f t="shared" si="0"/>
@@ -931,7 +925,7 @@
       <c r="E25" s="15"/>
       <c r="F25" s="12"/>
     </row>
-    <row r="26" spans="1:6" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="26" spans="1:6" customFormat="1" ht="16.5" customHeight="1">
       <c r="A26" s="3"/>
       <c r="C26" s="3" t="str">
         <f t="shared" si="0"/>
@@ -941,7 +935,7 @@
       <c r="E26" s="15"/>
       <c r="F26" s="12"/>
     </row>
-    <row r="27" spans="1:6" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="27" spans="1:6" customFormat="1" ht="16.5" customHeight="1">
       <c r="A27" s="3"/>
       <c r="C27" s="3" t="str">
         <f t="shared" si="0"/>
@@ -951,7 +945,7 @@
       <c r="E27" s="15"/>
       <c r="F27" s="12"/>
     </row>
-    <row r="28" spans="1:6" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="28" spans="1:6" customFormat="1" ht="16.5" customHeight="1">
       <c r="A28" s="3"/>
       <c r="C28" s="3" t="str">
         <f t="shared" si="0"/>
@@ -961,21 +955,21 @@
       <c r="E28" s="15"/>
       <c r="F28" s="12"/>
     </row>
-    <row r="29" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="29" spans="1:6" ht="16.5" customHeight="1">
       <c r="A29" s="8"/>
       <c r="C29" s="3" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
-    <row r="30" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="30" spans="1:6" ht="16.5" customHeight="1">
       <c r="A30" s="8"/>
       <c r="C30" s="3" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
-    <row r="31" spans="1:6" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="31" spans="1:6" customFormat="1" ht="16.5" customHeight="1">
       <c r="A31" s="3"/>
       <c r="C31" s="3" t="str">
         <f t="shared" si="0"/>
@@ -985,7 +979,7 @@
       <c r="E31" s="15"/>
       <c r="F31" s="12"/>
     </row>
-    <row r="32" spans="1:6" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="32" spans="1:6" customFormat="1" ht="16.5" customHeight="1">
       <c r="A32" s="3"/>
       <c r="C32" s="3" t="str">
         <f t="shared" si="0"/>
@@ -995,7 +989,7 @@
       <c r="E32" s="15"/>
       <c r="F32" s="12"/>
     </row>
-    <row r="33" spans="1:6" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="33" spans="1:6" customFormat="1" ht="16.5" customHeight="1">
       <c r="A33" s="3"/>
       <c r="C33" s="3" t="str">
         <f t="shared" si="0"/>
@@ -1005,7 +999,7 @@
       <c r="E33" s="15"/>
       <c r="F33" s="12"/>
     </row>
-    <row r="34" spans="1:6" customFormat="1" ht="53.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="34" spans="1:6" customFormat="1" ht="53.25" customHeight="1">
       <c r="A34" s="3"/>
       <c r="C34" s="3" t="str">
         <f t="shared" si="0"/>
@@ -1015,401 +1009,401 @@
       <c r="E34" s="15"/>
       <c r="F34" s="12"/>
     </row>
-    <row r="35" spans="1:6" ht="48.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="35" spans="1:6" ht="48.75" customHeight="1">
       <c r="A35" s="8"/>
     </row>
-    <row r="36" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="36" spans="1:6" ht="16.5" customHeight="1">
       <c r="A36" s="8"/>
     </row>
-    <row r="37" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="37" spans="1:6" ht="16.5" customHeight="1">
       <c r="A37" s="8"/>
     </row>
-    <row r="38" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="38" spans="1:6" ht="16.5" customHeight="1">
       <c r="A38" s="8"/>
     </row>
-    <row r="39" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="39" spans="1:6" ht="16.5" customHeight="1">
       <c r="A39" s="8"/>
     </row>
-    <row r="40" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="40" spans="1:6" ht="16.5" customHeight="1">
       <c r="A40" s="8"/>
     </row>
-    <row r="41" spans="1:6" ht="37.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="41" spans="1:6" ht="37.5" customHeight="1">
       <c r="A41" s="8"/>
     </row>
-    <row r="42" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="42" spans="1:6" ht="16.5" customHeight="1">
       <c r="A42" s="8"/>
     </row>
-    <row r="43" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="43" spans="1:6" ht="16.5" customHeight="1">
       <c r="A43" s="8"/>
     </row>
-    <row r="44" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="44" spans="1:6" ht="16.5" customHeight="1">
       <c r="A44" s="8"/>
     </row>
-    <row r="45" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="45" spans="1:6" ht="16.5" customHeight="1">
       <c r="A45" s="8"/>
     </row>
-    <row r="46" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="46" spans="1:6" ht="16.5" customHeight="1">
       <c r="A46" s="8"/>
     </row>
-    <row r="47" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="47" spans="1:6" ht="16.5" customHeight="1">
       <c r="A47" s="8"/>
     </row>
-    <row r="48" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="48" spans="1:6" ht="16.5" customHeight="1">
       <c r="A48" s="8"/>
     </row>
-    <row r="49" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="49" spans="1:1" ht="16.5" customHeight="1">
       <c r="A49" s="8"/>
     </row>
-    <row r="50" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="50" spans="1:1" ht="16.5" customHeight="1">
       <c r="A50" s="8"/>
     </row>
-    <row r="51" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="51" spans="1:1" ht="16.5" customHeight="1">
       <c r="A51" s="8"/>
     </row>
-    <row r="52" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="52" spans="1:1" ht="16.5" customHeight="1">
       <c r="A52" s="8"/>
     </row>
-    <row r="53" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="53" spans="1:1" ht="16.5" customHeight="1">
       <c r="A53" s="8"/>
     </row>
-    <row r="54" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="54" spans="1:1" ht="16.5" customHeight="1">
       <c r="A54" s="8"/>
     </row>
-    <row r="55" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="55" spans="1:1" ht="16.5" customHeight="1">
       <c r="A55" s="8"/>
     </row>
-    <row r="56" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="56" spans="1:1" ht="16.5" customHeight="1">
       <c r="A56" s="8"/>
     </row>
-    <row r="57" spans="1:1" ht="32.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="57" spans="1:1" ht="32.25" customHeight="1">
       <c r="A57" s="8"/>
     </row>
-    <row r="58" spans="1:1" ht="49.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="58" spans="1:1" ht="49.5" customHeight="1">
       <c r="A58" s="8"/>
     </row>
-    <row r="59" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="59" spans="1:1" ht="16.5" customHeight="1">
       <c r="A59" s="8"/>
     </row>
-    <row r="60" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="60" spans="1:1" ht="16.5" customHeight="1">
       <c r="A60" s="8"/>
     </row>
-    <row r="61" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="61" spans="1:1" ht="16.5" customHeight="1">
       <c r="A61" s="8"/>
     </row>
-    <row r="62" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="62" spans="1:1" ht="16.5" customHeight="1">
       <c r="A62" s="8"/>
     </row>
-    <row r="63" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="63" spans="1:1" ht="16.5" customHeight="1">
       <c r="A63" s="8"/>
     </row>
-    <row r="64" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="64" spans="1:1" ht="16.5" customHeight="1">
       <c r="A64" s="8"/>
     </row>
-    <row r="65" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="65" spans="1:1" ht="16.5" customHeight="1">
       <c r="A65" s="8"/>
     </row>
-    <row r="66" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="66" spans="1:1" ht="16.5" customHeight="1">
       <c r="A66" s="8"/>
     </row>
-    <row r="67" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="67" spans="1:1" ht="16.5" customHeight="1">
       <c r="A67" s="8"/>
     </row>
-    <row r="68" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="68" spans="1:1" ht="16.5" customHeight="1">
       <c r="A68" s="8"/>
     </row>
-    <row r="69" spans="1:1" ht="27.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="69" spans="1:1" ht="27.75" customHeight="1">
       <c r="A69" s="8"/>
     </row>
-    <row r="70" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="70" spans="1:1" ht="16.5" customHeight="1">
       <c r="A70" s="8"/>
     </row>
-    <row r="71" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="71" spans="1:1" ht="16.5" customHeight="1">
       <c r="A71" s="8"/>
     </row>
-    <row r="72" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="72" spans="1:1" ht="16.5" customHeight="1">
       <c r="A72" s="8"/>
     </row>
-    <row r="73" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="73" spans="1:1" ht="16.5" customHeight="1">
       <c r="A73" s="8"/>
     </row>
-    <row r="74" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="74" spans="1:1" ht="16.5" customHeight="1">
       <c r="A74" s="8"/>
     </row>
-    <row r="75" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="75" spans="1:1" ht="16.5" customHeight="1">
       <c r="A75" s="8"/>
     </row>
-    <row r="76" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="76" spans="1:1" ht="16.5" customHeight="1">
       <c r="A76" s="8"/>
     </row>
-    <row r="77" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="77" spans="1:1" ht="16.5" customHeight="1">
       <c r="A77" s="8"/>
     </row>
-    <row r="78" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="78" spans="1:1" ht="16.5" customHeight="1">
       <c r="A78" s="8"/>
     </row>
-    <row r="79" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="79" spans="1:1" ht="16.5" customHeight="1">
       <c r="A79" s="8"/>
     </row>
-    <row r="80" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="80" spans="1:1" ht="16.5" customHeight="1">
       <c r="A80" s="8"/>
     </row>
-    <row r="81" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="81" spans="1:1" ht="16.5" customHeight="1">
       <c r="A81" s="8"/>
     </row>
-    <row r="82" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="82" spans="1:1" ht="16.5" customHeight="1">
       <c r="A82" s="8"/>
     </row>
-    <row r="83" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="83" spans="1:1" ht="16.5" customHeight="1">
       <c r="A83" s="8"/>
     </row>
-    <row r="84" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="84" spans="1:1" ht="16.5" customHeight="1">
       <c r="A84" s="8"/>
     </row>
-    <row r="85" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="85" spans="1:1" ht="16.5" customHeight="1">
       <c r="A85" s="8"/>
     </row>
-    <row r="86" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="86" spans="1:1" ht="16.5" customHeight="1">
       <c r="A86" s="8"/>
     </row>
-    <row r="87" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="87" spans="1:1" ht="16.5" customHeight="1">
       <c r="A87" s="8"/>
     </row>
-    <row r="88" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="88" spans="1:1" ht="16.5" customHeight="1">
       <c r="A88" s="8"/>
     </row>
-    <row r="89" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="89" spans="1:1" ht="16.5" customHeight="1">
       <c r="A89" s="8"/>
     </row>
-    <row r="90" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="90" spans="1:1" ht="16.5" customHeight="1">
       <c r="A90" s="8"/>
     </row>
-    <row r="91" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="91" spans="1:1" ht="16.5" customHeight="1">
       <c r="A91" s="8"/>
     </row>
-    <row r="92" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="92" spans="1:1" ht="16.5" customHeight="1">
       <c r="A92" s="8"/>
     </row>
-    <row r="93" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="93" spans="1:1" ht="16.5" customHeight="1">
       <c r="A93" s="8"/>
     </row>
-    <row r="94" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="94" spans="1:1" ht="16.5" customHeight="1">
       <c r="A94" s="8"/>
     </row>
-    <row r="95" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="95" spans="1:1" ht="16.5" customHeight="1">
       <c r="A95" s="8"/>
     </row>
-    <row r="96" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="96" spans="1:1" ht="16.5" customHeight="1">
       <c r="A96" s="8"/>
     </row>
-    <row r="97" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="97" spans="1:1" ht="16.5" customHeight="1">
       <c r="A97" s="8"/>
     </row>
-    <row r="98" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="98" spans="1:1" ht="16.5" customHeight="1">
       <c r="A98" s="8"/>
     </row>
-    <row r="99" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="99" spans="1:1" ht="16.5" customHeight="1">
       <c r="A99" s="8"/>
     </row>
-    <row r="100" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="100" spans="1:1" ht="16.5" customHeight="1">
       <c r="A100" s="8"/>
     </row>
-    <row r="101" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="101" spans="1:1" ht="16.5" customHeight="1">
       <c r="A101" s="8"/>
     </row>
-    <row r="102" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="102" spans="1:1" ht="16.5" customHeight="1">
       <c r="A102" s="8"/>
     </row>
-    <row r="103" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="103" spans="1:1" ht="16.5" customHeight="1">
       <c r="A103" s="8"/>
     </row>
-    <row r="104" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="104" spans="1:1" ht="16.5" customHeight="1">
       <c r="A104" s="8"/>
     </row>
-    <row r="105" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="105" spans="1:1" ht="16.5" customHeight="1">
       <c r="A105" s="8"/>
     </row>
-    <row r="106" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="106" spans="1:1" ht="16.5" customHeight="1">
       <c r="A106" s="8"/>
     </row>
-    <row r="107" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="107" spans="1:1" ht="16.5" customHeight="1">
       <c r="A107" s="8"/>
     </row>
-    <row r="108" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="108" spans="1:1" ht="16.5" customHeight="1">
       <c r="A108" s="8"/>
     </row>
-    <row r="109" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="109" spans="1:1" ht="16.5" customHeight="1">
       <c r="A109" s="8"/>
     </row>
-    <row r="110" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="110" spans="1:1" ht="16.5" customHeight="1">
       <c r="A110" s="8"/>
     </row>
-    <row r="111" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="111" spans="1:1" ht="16.5" customHeight="1">
       <c r="A111" s="8"/>
     </row>
-    <row r="112" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="112" spans="1:1" ht="16.5" customHeight="1">
       <c r="A112" s="8"/>
     </row>
-    <row r="113" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="113" spans="1:1" ht="16.5" customHeight="1">
       <c r="A113" s="8"/>
     </row>
-    <row r="114" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="114" spans="1:1" ht="16.5" customHeight="1">
       <c r="A114" s="8"/>
     </row>
-    <row r="115" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="115" spans="1:1" ht="16.5" customHeight="1">
       <c r="A115" s="8"/>
     </row>
-    <row r="116" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="116" spans="1:1" ht="16.5" customHeight="1">
       <c r="A116" s="8"/>
     </row>
-    <row r="117" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="117" spans="1:1" ht="16.5" customHeight="1">
       <c r="A117" s="8"/>
     </row>
-    <row r="118" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="118" spans="1:1" ht="16.5" customHeight="1">
       <c r="A118" s="8"/>
     </row>
-    <row r="119" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="119" spans="1:1" ht="16.5" customHeight="1">
       <c r="A119" s="8"/>
     </row>
-    <row r="120" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="120" spans="1:1" ht="16.5" customHeight="1">
       <c r="A120" s="8"/>
     </row>
-    <row r="121" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="121" spans="1:1" ht="16.5" customHeight="1">
       <c r="A121" s="8"/>
     </row>
-    <row r="122" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="122" spans="1:1" ht="16.5" customHeight="1">
       <c r="A122" s="8"/>
     </row>
-    <row r="123" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="123" spans="1:1" ht="16.5" customHeight="1">
       <c r="A123" s="8"/>
     </row>
-    <row r="124" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="124" spans="1:1" ht="16.5" customHeight="1">
       <c r="A124" s="8"/>
     </row>
-    <row r="125" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="125" spans="1:1" ht="16.5" customHeight="1">
       <c r="A125" s="8"/>
     </row>
-    <row r="126" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="126" spans="1:1" ht="16.5" customHeight="1">
       <c r="A126" s="8"/>
     </row>
-    <row r="127" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="127" spans="1:1" ht="16.5" customHeight="1">
       <c r="A127" s="8"/>
     </row>
-    <row r="128" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="128" spans="1:1" ht="16.5" customHeight="1">
       <c r="A128" s="8"/>
     </row>
-    <row r="129" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="129" spans="1:1" ht="16.5" customHeight="1">
       <c r="A129" s="8"/>
     </row>
-    <row r="130" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="130" spans="1:1" ht="16.5" customHeight="1">
       <c r="A130" s="8"/>
     </row>
-    <row r="131" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="131" spans="1:1" ht="16.5" customHeight="1">
       <c r="A131" s="8"/>
     </row>
-    <row r="132" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="132" spans="1:1" ht="16.5" customHeight="1">
       <c r="A132" s="8"/>
     </row>
-    <row r="133" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="133" spans="1:1" ht="16.5" customHeight="1">
       <c r="A133" s="8"/>
     </row>
-    <row r="134" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="134" spans="1:1" ht="16.5" customHeight="1">
       <c r="A134" s="8"/>
     </row>
-    <row r="135" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="135" spans="1:1" ht="16.5" customHeight="1">
       <c r="A135" s="8"/>
     </row>
-    <row r="136" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="136" spans="1:1" ht="16.5" customHeight="1">
       <c r="A136" s="8"/>
     </row>
-    <row r="137" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="137" spans="1:1" ht="16.5" customHeight="1">
       <c r="A137" s="8"/>
     </row>
-    <row r="138" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="138" spans="1:1" ht="16.5" customHeight="1">
       <c r="A138" s="8"/>
     </row>
-    <row r="139" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="139" spans="1:1" ht="16.5" customHeight="1">
       <c r="A139" s="8"/>
     </row>
-    <row r="140" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="140" spans="1:1" ht="16.5" customHeight="1">
       <c r="A140" s="8"/>
     </row>
-    <row r="141" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="141" spans="1:1" ht="16.5" customHeight="1">
       <c r="A141" s="8"/>
     </row>
-    <row r="142" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="142" spans="1:1" ht="16.5" customHeight="1">
       <c r="A142" s="8"/>
     </row>
-    <row r="143" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="143" spans="1:1" ht="16.5" customHeight="1">
       <c r="A143" s="8"/>
     </row>
-    <row r="144" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="144" spans="1:1" ht="16.5" customHeight="1">
       <c r="A144" s="8"/>
     </row>
-    <row r="145" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="145" spans="1:1" ht="16.5" customHeight="1">
       <c r="A145" s="8"/>
     </row>
-    <row r="146" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="146" spans="1:1" ht="16.5" customHeight="1">
       <c r="A146" s="8"/>
     </row>
-    <row r="147" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="147" spans="1:1" ht="16.5" customHeight="1">
       <c r="A147" s="8"/>
     </row>
-    <row r="148" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="148" spans="1:1" ht="16.5" customHeight="1">
       <c r="A148" s="8"/>
     </row>
-    <row r="149" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="149" spans="1:1" ht="16.5" customHeight="1">
       <c r="A149" s="8"/>
     </row>
-    <row r="150" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="150" spans="1:1" ht="16.5" customHeight="1">
       <c r="A150" s="8"/>
     </row>
-    <row r="151" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="151" spans="1:1" ht="16.5" customHeight="1">
       <c r="A151" s="8"/>
     </row>
-    <row r="152" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="152" spans="1:1" ht="16.5" customHeight="1">
       <c r="A152" s="8"/>
     </row>
-    <row r="153" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="153" spans="1:1" ht="16.5" customHeight="1">
       <c r="A153" s="8"/>
     </row>
-    <row r="154" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="154" spans="1:1" ht="16.5" customHeight="1">
       <c r="A154" s="8"/>
     </row>
-    <row r="155" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="155" spans="1:1" ht="16.5" customHeight="1">
       <c r="A155" s="8"/>
     </row>
-    <row r="156" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="156" spans="1:1" ht="16.5" customHeight="1">
       <c r="A156" s="8"/>
     </row>
-    <row r="157" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="157" spans="1:1" ht="16.5" customHeight="1">
       <c r="A157" s="8"/>
     </row>
-    <row r="158" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="158" spans="1:1" ht="16.5" customHeight="1">
       <c r="A158" s="8"/>
     </row>
-    <row r="159" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="159" spans="1:1" ht="16.5" customHeight="1">
       <c r="A159" s="8"/>
     </row>
-    <row r="160" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="160" spans="1:1" ht="16.5" customHeight="1">
       <c r="A160" s="8"/>
     </row>
-    <row r="161" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="161" spans="1:1" ht="16.5" customHeight="1">
       <c r="A161" s="8"/>
     </row>
-    <row r="162" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="162" spans="1:1" ht="16.5" customHeight="1">
       <c r="A162" s="8"/>
     </row>
-    <row r="163" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="163" spans="1:1" ht="16.5" customHeight="1">
       <c r="A163" s="8"/>
     </row>
-    <row r="164" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="164" spans="1:1" ht="16.5" customHeight="1">
       <c r="A164" s="8"/>
     </row>
-    <row r="165" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="165" spans="1:1" ht="16.5" customHeight="1">
       <c r="A165" s="8"/>
     </row>
   </sheetData>
-  <autoFilter ref="B1:F69" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
+  <autoFilter ref="B1:F69"/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -1418,14 +1412,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:F167"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5" customHeight="1" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultRowHeight="16.5" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="1.6640625" style="14" customWidth="1"/>
     <col min="2" max="2" width="59.21875" style="1" customWidth="1"/>
@@ -1435,7 +1429,7 @@
     <col min="6" max="6" width="50.21875" style="12" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="30.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:6" ht="30.75" customHeight="1">
       <c r="A1" s="2"/>
       <c r="B1" s="5" t="s">
         <v>3</v>
@@ -1453,7 +1447,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:6" ht="16.5" customHeight="1">
       <c r="A2" s="3"/>
       <c r="B2" t="s">
         <v>16</v>
@@ -1469,7 +1463,7 @@
         <v>45777</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:6" ht="16.5" customHeight="1">
       <c r="A3" s="3"/>
       <c r="B3" s="17" t="s">
         <v>15</v>
@@ -1485,7 +1479,7 @@
         <v>45777</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:6" ht="16.5" customHeight="1">
       <c r="A4" s="3"/>
       <c r="B4" t="s">
         <v>21</v>
@@ -1501,14 +1495,14 @@
         <v>45779</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:6" ht="16.5" customHeight="1">
       <c r="A5" s="3"/>
       <c r="C5" s="3" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="33.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:6" ht="33.75" customHeight="1">
       <c r="A6" s="3"/>
       <c r="B6"/>
       <c r="C6" s="3" t="str">
@@ -1518,7 +1512,7 @@
       <c r="D6" s="15"/>
       <c r="E6" s="15"/>
     </row>
-    <row r="7" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:6" ht="16.5" customHeight="1">
       <c r="A7" s="3"/>
       <c r="B7"/>
       <c r="C7" s="3" t="str">
@@ -1528,7 +1522,7 @@
       <c r="D7" s="15"/>
       <c r="E7" s="15"/>
     </row>
-    <row r="8" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:6" ht="16.5" customHeight="1">
       <c r="A8" s="3"/>
       <c r="C8" s="3" t="str">
         <f t="shared" si="0"/>
@@ -1537,7 +1531,7 @@
       <c r="D8" s="15"/>
       <c r="E8" s="15"/>
     </row>
-    <row r="9" spans="1:6" ht="13.5" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:6" ht="13.5">
       <c r="A9" s="3"/>
       <c r="B9"/>
       <c r="C9" s="3" t="str">
@@ -1547,7 +1541,7 @@
       <c r="D9" s="15"/>
       <c r="E9" s="15"/>
     </row>
-    <row r="10" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:6" ht="16.5" customHeight="1">
       <c r="A10" s="3"/>
       <c r="B10"/>
       <c r="C10" s="3" t="str">
@@ -1557,14 +1551,14 @@
       <c r="D10" s="15"/>
       <c r="E10" s="15"/>
     </row>
-    <row r="11" spans="1:6" ht="36.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:6" ht="36.75" customHeight="1">
       <c r="A11" s="3"/>
       <c r="C11" s="3" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
-    <row r="12" spans="1:6" ht="32.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:6" ht="32.25" customHeight="1">
       <c r="A12" s="3"/>
       <c r="B12"/>
       <c r="C12" s="3" t="str">
@@ -1574,7 +1568,7 @@
       <c r="D12" s="15"/>
       <c r="E12" s="15"/>
     </row>
-    <row r="13" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:6" ht="16.5" customHeight="1">
       <c r="A13" s="3"/>
       <c r="B13"/>
       <c r="C13" s="3" t="str">
@@ -1584,7 +1578,7 @@
       <c r="D13" s="15"/>
       <c r="E13" s="15"/>
     </row>
-    <row r="14" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:6" ht="16.5" customHeight="1">
       <c r="A14" s="3"/>
       <c r="B14"/>
       <c r="C14" s="3" t="str">
@@ -1594,7 +1588,7 @@
       <c r="D14" s="15"/>
       <c r="E14" s="15"/>
     </row>
-    <row r="15" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:6" ht="16.5" customHeight="1">
       <c r="A15" s="3"/>
       <c r="B15"/>
       <c r="C15" s="3" t="str">
@@ -1604,7 +1598,7 @@
       <c r="D15" s="15"/>
       <c r="E15" s="15"/>
     </row>
-    <row r="16" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:6" ht="16.5" customHeight="1">
       <c r="A16" s="3"/>
       <c r="B16"/>
       <c r="C16" s="3" t="str">
@@ -1614,14 +1608,14 @@
       <c r="D16" s="15"/>
       <c r="E16" s="15"/>
     </row>
-    <row r="17" spans="1:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:5" ht="16.5" customHeight="1">
       <c r="A17" s="3"/>
       <c r="C17" s="3" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
-    <row r="18" spans="1:5" ht="39" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:5" ht="39" customHeight="1">
       <c r="A18" s="3"/>
       <c r="B18"/>
       <c r="C18" s="3" t="str">
@@ -1631,7 +1625,7 @@
       <c r="D18" s="15"/>
       <c r="E18" s="15"/>
     </row>
-    <row r="19" spans="1:5" ht="45.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:5" ht="45.75" customHeight="1">
       <c r="A19" s="3"/>
       <c r="B19"/>
       <c r="C19" s="3" t="str">
@@ -1641,7 +1635,7 @@
       <c r="D19" s="15"/>
       <c r="E19" s="15"/>
     </row>
-    <row r="20" spans="1:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:5" ht="16.5" customHeight="1">
       <c r="A20" s="3"/>
       <c r="B20"/>
       <c r="C20" s="3" t="str">
@@ -1651,7 +1645,7 @@
       <c r="D20" s="15"/>
       <c r="E20" s="15"/>
     </row>
-    <row r="21" spans="1:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:5" ht="16.5" customHeight="1">
       <c r="A21" s="3"/>
       <c r="B21"/>
       <c r="C21" s="3" t="str">
@@ -1661,7 +1655,7 @@
       <c r="D21" s="15"/>
       <c r="E21" s="15"/>
     </row>
-    <row r="22" spans="1:5" ht="13.5" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:5" ht="13.5">
       <c r="A22" s="3"/>
       <c r="B22"/>
       <c r="C22" s="3" t="str">
@@ -1671,14 +1665,14 @@
       <c r="D22" s="15"/>
       <c r="E22" s="15"/>
     </row>
-    <row r="23" spans="1:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:5" ht="16.5" customHeight="1">
       <c r="A23" s="3"/>
       <c r="C23" s="3" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
-    <row r="24" spans="1:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="24" spans="1:5" ht="16.5" customHeight="1">
       <c r="A24" s="3"/>
       <c r="B24"/>
       <c r="C24" s="3" t="str">
@@ -1688,7 +1682,7 @@
       <c r="D24" s="15"/>
       <c r="E24" s="15"/>
     </row>
-    <row r="25" spans="1:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="25" spans="1:5" ht="16.5" customHeight="1">
       <c r="A25" s="3"/>
       <c r="B25"/>
       <c r="C25" s="3" t="str">
@@ -1698,7 +1692,7 @@
       <c r="D25" s="15"/>
       <c r="E25" s="15"/>
     </row>
-    <row r="26" spans="1:5" ht="34.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="26" spans="1:5" ht="34.5" customHeight="1">
       <c r="A26" s="3"/>
       <c r="B26"/>
       <c r="C26" s="3" t="str">
@@ -1708,7 +1702,7 @@
       <c r="D26" s="15"/>
       <c r="E26" s="15"/>
     </row>
-    <row r="27" spans="1:5" ht="29.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="27" spans="1:5" ht="29.25" customHeight="1">
       <c r="A27" s="3"/>
       <c r="B27"/>
       <c r="C27" s="3" t="str">
@@ -1718,7 +1712,7 @@
       <c r="D27" s="15"/>
       <c r="E27" s="15"/>
     </row>
-    <row r="28" spans="1:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="28" spans="1:5" ht="16.5" customHeight="1">
       <c r="A28" s="3"/>
       <c r="B28"/>
       <c r="C28" s="3" t="str">
@@ -1728,21 +1722,21 @@
       <c r="D28" s="15"/>
       <c r="E28" s="15"/>
     </row>
-    <row r="29" spans="1:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="29" spans="1:5" ht="16.5" customHeight="1">
       <c r="A29" s="3"/>
       <c r="C29" s="3" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
-    <row r="30" spans="1:5" ht="36.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="30" spans="1:5" ht="36.75" customHeight="1">
       <c r="A30" s="3"/>
       <c r="C30" s="3" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
-    <row r="31" spans="1:5" ht="54.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="31" spans="1:5" ht="54.75" customHeight="1">
       <c r="A31" s="3"/>
       <c r="B31"/>
       <c r="C31" s="3" t="str">
@@ -1752,7 +1746,7 @@
       <c r="D31" s="15"/>
       <c r="E31" s="15"/>
     </row>
-    <row r="32" spans="1:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="32" spans="1:5" ht="16.5" customHeight="1">
       <c r="A32" s="3"/>
       <c r="B32"/>
       <c r="C32" s="3" t="str">
@@ -1762,7 +1756,7 @@
       <c r="D32" s="15"/>
       <c r="E32" s="15"/>
     </row>
-    <row r="33" spans="1:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="33" spans="1:5" ht="16.5" customHeight="1">
       <c r="A33" s="3"/>
       <c r="B33"/>
       <c r="C33" s="3" t="str">
@@ -1772,7 +1766,7 @@
       <c r="D33" s="15"/>
       <c r="E33" s="15"/>
     </row>
-    <row r="34" spans="1:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="34" spans="1:5" ht="16.5" customHeight="1">
       <c r="A34" s="3"/>
       <c r="B34"/>
       <c r="C34" s="3" t="str">
@@ -1782,467 +1776,467 @@
       <c r="D34" s="15"/>
       <c r="E34" s="15"/>
     </row>
-    <row r="35" spans="1:5" ht="34.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="35" spans="1:5" ht="34.5" customHeight="1">
       <c r="A35" s="3"/>
       <c r="C35" s="3" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
-    <row r="36" spans="1:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="36" spans="1:5" ht="16.5" customHeight="1">
       <c r="A36" s="3"/>
       <c r="C36" s="3" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
-    <row r="37" spans="1:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="37" spans="1:5" ht="16.5" customHeight="1">
       <c r="A37" s="3"/>
       <c r="C37" s="3" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
-    <row r="38" spans="1:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="38" spans="1:5" ht="16.5" customHeight="1">
       <c r="A38" s="3"/>
       <c r="C38" s="3" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
-    <row r="39" spans="1:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="39" spans="1:5" ht="16.5" customHeight="1">
       <c r="A39" s="3"/>
       <c r="C39" s="3" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
-    <row r="40" spans="1:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="40" spans="1:5" ht="16.5" customHeight="1">
       <c r="A40" s="3"/>
       <c r="C40" s="3" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
-    <row r="41" spans="1:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="41" spans="1:5" ht="16.5" customHeight="1">
       <c r="A41" s="3"/>
       <c r="C41" s="3" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
-    <row r="42" spans="1:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="42" spans="1:5" ht="16.5" customHeight="1">
       <c r="A42" s="3"/>
       <c r="C42" s="3" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
-    <row r="43" spans="1:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="43" spans="1:5" ht="16.5" customHeight="1">
       <c r="A43" s="3"/>
       <c r="C43" s="3" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
-    <row r="44" spans="1:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="44" spans="1:5" ht="16.5" customHeight="1">
       <c r="A44" s="3"/>
       <c r="C44" s="3" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
-    <row r="45" spans="1:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="45" spans="1:5" ht="16.5" customHeight="1">
       <c r="A45" s="3"/>
       <c r="C45" s="3" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
-    <row r="46" spans="1:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="46" spans="1:5" ht="16.5" customHeight="1">
       <c r="A46" s="3"/>
       <c r="C46" s="3" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
-    <row r="47" spans="1:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="47" spans="1:5" ht="16.5" customHeight="1">
       <c r="A47" s="3"/>
       <c r="C47" s="3" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
-    <row r="48" spans="1:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="48" spans="1:5" ht="16.5" customHeight="1">
       <c r="A48" s="3"/>
       <c r="C48" s="3" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
-    <row r="49" spans="1:3" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="49" spans="1:3" ht="16.5" customHeight="1">
       <c r="A49" s="3"/>
       <c r="C49" s="3" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
-    <row r="50" spans="1:3" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="50" spans="1:3" ht="16.5" customHeight="1">
       <c r="A50" s="3"/>
     </row>
-    <row r="51" spans="1:3" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="51" spans="1:3" ht="16.5" customHeight="1">
       <c r="A51" s="3"/>
     </row>
-    <row r="52" spans="1:3" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="52" spans="1:3" ht="16.5" customHeight="1">
       <c r="A52" s="3"/>
     </row>
-    <row r="53" spans="1:3" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="53" spans="1:3" ht="16.5" customHeight="1">
       <c r="A53" s="3"/>
     </row>
-    <row r="54" spans="1:3" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="54" spans="1:3" ht="16.5" customHeight="1">
       <c r="A54" s="3"/>
     </row>
-    <row r="55" spans="1:3" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="55" spans="1:3" ht="16.5" customHeight="1">
       <c r="A55" s="3"/>
     </row>
-    <row r="56" spans="1:3" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="56" spans="1:3" ht="16.5" customHeight="1">
       <c r="A56" s="3"/>
     </row>
-    <row r="57" spans="1:3" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="57" spans="1:3" ht="16.5" customHeight="1">
       <c r="A57" s="3"/>
     </row>
-    <row r="58" spans="1:3" ht="13.5" x14ac:dyDescent="0.15">
+    <row r="58" spans="1:3" ht="13.5">
       <c r="A58" s="3"/>
     </row>
-    <row r="59" spans="1:3" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="59" spans="1:3" ht="16.5" customHeight="1">
       <c r="A59" s="3"/>
     </row>
-    <row r="60" spans="1:3" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="60" spans="1:3" ht="16.5" customHeight="1">
       <c r="A60" s="3"/>
     </row>
-    <row r="61" spans="1:3" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="61" spans="1:3" ht="16.5" customHeight="1">
       <c r="A61" s="3"/>
     </row>
-    <row r="62" spans="1:3" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="62" spans="1:3" ht="16.5" customHeight="1">
       <c r="A62" s="3"/>
     </row>
-    <row r="63" spans="1:3" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="63" spans="1:3" ht="16.5" customHeight="1">
       <c r="A63" s="3"/>
     </row>
-    <row r="64" spans="1:3" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="64" spans="1:3" ht="16.5" customHeight="1">
       <c r="A64" s="3"/>
     </row>
-    <row r="65" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="65" spans="1:1" ht="16.5" customHeight="1">
       <c r="A65" s="3"/>
     </row>
-    <row r="66" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="66" spans="1:1" ht="16.5" customHeight="1">
       <c r="A66" s="3"/>
     </row>
-    <row r="67" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="67" spans="1:1" ht="16.5" customHeight="1">
       <c r="A67" s="3"/>
     </row>
-    <row r="68" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="68" spans="1:1" ht="16.5" customHeight="1">
       <c r="A68" s="3"/>
     </row>
-    <row r="69" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="69" spans="1:1" ht="16.5" customHeight="1">
       <c r="A69" s="3"/>
     </row>
-    <row r="70" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="70" spans="1:1" ht="16.5" customHeight="1">
       <c r="A70" s="3"/>
     </row>
-    <row r="71" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="71" spans="1:1" ht="16.5" customHeight="1">
       <c r="A71" s="3"/>
     </row>
-    <row r="72" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="72" spans="1:1" ht="16.5" customHeight="1">
       <c r="A72" s="3"/>
     </row>
-    <row r="73" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="73" spans="1:1" ht="16.5" customHeight="1">
       <c r="A73" s="3"/>
     </row>
-    <row r="74" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="74" spans="1:1" ht="16.5" customHeight="1">
       <c r="A74" s="3"/>
     </row>
-    <row r="75" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="75" spans="1:1" ht="16.5" customHeight="1">
       <c r="A75" s="3"/>
     </row>
-    <row r="76" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="76" spans="1:1" ht="16.5" customHeight="1">
       <c r="A76" s="3"/>
     </row>
-    <row r="77" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="77" spans="1:1" ht="16.5" customHeight="1">
       <c r="A77" s="3"/>
     </row>
-    <row r="78" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="78" spans="1:1" ht="16.5" customHeight="1">
       <c r="A78" s="3"/>
     </row>
-    <row r="79" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="79" spans="1:1" ht="16.5" customHeight="1">
       <c r="A79" s="3"/>
     </row>
-    <row r="80" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="80" spans="1:1" ht="16.5" customHeight="1">
       <c r="A80" s="3"/>
     </row>
-    <row r="81" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="81" spans="1:1" ht="16.5" customHeight="1">
       <c r="A81" s="3"/>
     </row>
-    <row r="82" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="82" spans="1:1" ht="16.5" customHeight="1">
       <c r="A82" s="3"/>
     </row>
-    <row r="83" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="83" spans="1:1" ht="16.5" customHeight="1">
       <c r="A83" s="3"/>
     </row>
-    <row r="84" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="84" spans="1:1" ht="16.5" customHeight="1">
       <c r="A84" s="3"/>
     </row>
-    <row r="85" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="85" spans="1:1" ht="16.5" customHeight="1">
       <c r="A85" s="3"/>
     </row>
-    <row r="86" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="86" spans="1:1" ht="16.5" customHeight="1">
       <c r="A86" s="3"/>
     </row>
-    <row r="87" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="87" spans="1:1" ht="16.5" customHeight="1">
       <c r="A87" s="3"/>
     </row>
-    <row r="88" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="88" spans="1:1" ht="16.5" customHeight="1">
       <c r="A88" s="3"/>
     </row>
-    <row r="89" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="89" spans="1:1" ht="16.5" customHeight="1">
       <c r="A89" s="3"/>
     </row>
-    <row r="90" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="90" spans="1:1" ht="16.5" customHeight="1">
       <c r="A90" s="3"/>
     </row>
-    <row r="91" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="91" spans="1:1" ht="16.5" customHeight="1">
       <c r="A91" s="3"/>
     </row>
-    <row r="92" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="92" spans="1:1" ht="16.5" customHeight="1">
       <c r="A92" s="3"/>
     </row>
-    <row r="93" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="93" spans="1:1" ht="16.5" customHeight="1">
       <c r="A93" s="3"/>
     </row>
-    <row r="94" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="94" spans="1:1" ht="16.5" customHeight="1">
       <c r="A94" s="3"/>
     </row>
-    <row r="95" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="95" spans="1:1" ht="16.5" customHeight="1">
       <c r="A95" s="3"/>
     </row>
-    <row r="96" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="96" spans="1:1" ht="16.5" customHeight="1">
       <c r="A96" s="3"/>
     </row>
-    <row r="97" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="97" spans="1:1" ht="16.5" customHeight="1">
       <c r="A97" s="3"/>
     </row>
-    <row r="98" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="98" spans="1:1" ht="16.5" customHeight="1">
       <c r="A98" s="3"/>
     </row>
-    <row r="99" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="99" spans="1:1" ht="16.5" customHeight="1">
       <c r="A99" s="3"/>
     </row>
-    <row r="100" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="100" spans="1:1" ht="16.5" customHeight="1">
       <c r="A100" s="3"/>
     </row>
-    <row r="101" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="101" spans="1:1" ht="16.5" customHeight="1">
       <c r="A101" s="3"/>
     </row>
-    <row r="102" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="102" spans="1:1" ht="16.5" customHeight="1">
       <c r="A102" s="3"/>
     </row>
-    <row r="103" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="103" spans="1:1" ht="16.5" customHeight="1">
       <c r="A103" s="3"/>
     </row>
-    <row r="104" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="104" spans="1:1" ht="16.5" customHeight="1">
       <c r="A104" s="3"/>
     </row>
-    <row r="105" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="105" spans="1:1" ht="16.5" customHeight="1">
       <c r="A105" s="3"/>
     </row>
-    <row r="106" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="106" spans="1:1" ht="16.5" customHeight="1">
       <c r="A106" s="3"/>
     </row>
-    <row r="107" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="107" spans="1:1" ht="16.5" customHeight="1">
       <c r="A107" s="3"/>
     </row>
-    <row r="108" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="108" spans="1:1" ht="16.5" customHeight="1">
       <c r="A108" s="3"/>
     </row>
-    <row r="109" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="109" spans="1:1" ht="16.5" customHeight="1">
       <c r="A109" s="3"/>
     </row>
-    <row r="110" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="110" spans="1:1" ht="16.5" customHeight="1">
       <c r="A110" s="3"/>
     </row>
-    <row r="111" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="111" spans="1:1" ht="16.5" customHeight="1">
       <c r="A111" s="3"/>
     </row>
-    <row r="112" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="112" spans="1:1" ht="16.5" customHeight="1">
       <c r="A112" s="3"/>
     </row>
-    <row r="113" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="113" spans="1:1" ht="16.5" customHeight="1">
       <c r="A113" s="3"/>
     </row>
-    <row r="114" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="114" spans="1:1" ht="16.5" customHeight="1">
       <c r="A114" s="3"/>
     </row>
-    <row r="115" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="115" spans="1:1" ht="16.5" customHeight="1">
       <c r="A115" s="3"/>
     </row>
-    <row r="116" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="116" spans="1:1" ht="16.5" customHeight="1">
       <c r="A116" s="3"/>
     </row>
-    <row r="117" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="117" spans="1:1" ht="16.5" customHeight="1">
       <c r="A117" s="3"/>
     </row>
-    <row r="118" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="118" spans="1:1" ht="16.5" customHeight="1">
       <c r="A118" s="3"/>
     </row>
-    <row r="119" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="119" spans="1:1" ht="16.5" customHeight="1">
       <c r="A119" s="3"/>
     </row>
-    <row r="120" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="120" spans="1:1" ht="16.5" customHeight="1">
       <c r="A120" s="3"/>
     </row>
-    <row r="121" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="121" spans="1:1" ht="16.5" customHeight="1">
       <c r="A121" s="3"/>
     </row>
-    <row r="122" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="122" spans="1:1" ht="16.5" customHeight="1">
       <c r="A122" s="3"/>
     </row>
-    <row r="123" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="123" spans="1:1" ht="16.5" customHeight="1">
       <c r="A123" s="3"/>
     </row>
-    <row r="124" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="124" spans="1:1" ht="16.5" customHeight="1">
       <c r="A124" s="3"/>
     </row>
-    <row r="125" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="125" spans="1:1" ht="16.5" customHeight="1">
       <c r="A125" s="3"/>
     </row>
-    <row r="126" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="126" spans="1:1" ht="16.5" customHeight="1">
       <c r="A126" s="3"/>
     </row>
-    <row r="127" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="127" spans="1:1" ht="16.5" customHeight="1">
       <c r="A127" s="3"/>
     </row>
-    <row r="128" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="128" spans="1:1" ht="16.5" customHeight="1">
       <c r="A128" s="3"/>
     </row>
-    <row r="129" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="129" spans="1:1" ht="16.5" customHeight="1">
       <c r="A129" s="3"/>
     </row>
-    <row r="130" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="130" spans="1:1" ht="16.5" customHeight="1">
       <c r="A130" s="3"/>
     </row>
-    <row r="131" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="131" spans="1:1" ht="16.5" customHeight="1">
       <c r="A131" s="3"/>
     </row>
-    <row r="132" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="132" spans="1:1" ht="16.5" customHeight="1">
       <c r="A132" s="3"/>
     </row>
-    <row r="133" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="133" spans="1:1" ht="16.5" customHeight="1">
       <c r="A133" s="3"/>
     </row>
-    <row r="134" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="134" spans="1:1" ht="16.5" customHeight="1">
       <c r="A134" s="3"/>
     </row>
-    <row r="135" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="135" spans="1:1" ht="16.5" customHeight="1">
       <c r="A135" s="3"/>
     </row>
-    <row r="136" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="136" spans="1:1" ht="16.5" customHeight="1">
       <c r="A136" s="3"/>
     </row>
-    <row r="137" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="137" spans="1:1" ht="16.5" customHeight="1">
       <c r="A137" s="3"/>
     </row>
-    <row r="138" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="138" spans="1:1" ht="16.5" customHeight="1">
       <c r="A138" s="3"/>
     </row>
-    <row r="139" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="139" spans="1:1" ht="16.5" customHeight="1">
       <c r="A139" s="3"/>
     </row>
-    <row r="140" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="140" spans="1:1" ht="16.5" customHeight="1">
       <c r="A140" s="3"/>
     </row>
-    <row r="141" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="141" spans="1:1" ht="16.5" customHeight="1">
       <c r="A141" s="3"/>
     </row>
-    <row r="142" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="142" spans="1:1" ht="16.5" customHeight="1">
       <c r="A142" s="3"/>
     </row>
-    <row r="143" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="143" spans="1:1" ht="16.5" customHeight="1">
       <c r="A143" s="3"/>
     </row>
-    <row r="144" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="144" spans="1:1" ht="16.5" customHeight="1">
       <c r="A144" s="3"/>
     </row>
-    <row r="145" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="145" spans="1:1" ht="16.5" customHeight="1">
       <c r="A145" s="3"/>
     </row>
-    <row r="146" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="146" spans="1:1" ht="16.5" customHeight="1">
       <c r="A146" s="3"/>
     </row>
-    <row r="147" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="147" spans="1:1" ht="16.5" customHeight="1">
       <c r="A147" s="3"/>
     </row>
-    <row r="148" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="148" spans="1:1" ht="16.5" customHeight="1">
       <c r="A148" s="3"/>
     </row>
-    <row r="149" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="149" spans="1:1" ht="16.5" customHeight="1">
       <c r="A149" s="3"/>
     </row>
-    <row r="150" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="150" spans="1:1" ht="16.5" customHeight="1">
       <c r="A150" s="3"/>
     </row>
-    <row r="151" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="151" spans="1:1" ht="16.5" customHeight="1">
       <c r="A151" s="3"/>
     </row>
-    <row r="152" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="152" spans="1:1" ht="16.5" customHeight="1">
       <c r="A152" s="3"/>
     </row>
-    <row r="153" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="153" spans="1:1" ht="16.5" customHeight="1">
       <c r="A153" s="3"/>
     </row>
-    <row r="154" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="154" spans="1:1" ht="16.5" customHeight="1">
       <c r="A154" s="3"/>
     </row>
-    <row r="155" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="155" spans="1:1" ht="16.5" customHeight="1">
       <c r="A155" s="3"/>
     </row>
-    <row r="156" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="156" spans="1:1" ht="16.5" customHeight="1">
       <c r="A156" s="3"/>
     </row>
-    <row r="157" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="157" spans="1:1" ht="16.5" customHeight="1">
       <c r="A157" s="3"/>
     </row>
-    <row r="158" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="158" spans="1:1" ht="16.5" customHeight="1">
       <c r="A158" s="3"/>
     </row>
-    <row r="159" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="159" spans="1:1" ht="16.5" customHeight="1">
       <c r="A159" s="3"/>
     </row>
-    <row r="160" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="160" spans="1:1" ht="16.5" customHeight="1">
       <c r="A160" s="3"/>
     </row>
-    <row r="161" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="161" spans="1:1" ht="16.5" customHeight="1">
       <c r="A161" s="3"/>
     </row>
-    <row r="162" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="162" spans="1:1" ht="16.5" customHeight="1">
       <c r="A162" s="3"/>
     </row>
-    <row r="163" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="163" spans="1:1" ht="16.5" customHeight="1">
       <c r="A163" s="3"/>
     </row>
-    <row r="164" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="164" spans="1:1" ht="16.5" customHeight="1">
       <c r="A164" s="3"/>
     </row>
-    <row r="165" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="165" spans="1:1" ht="16.5" customHeight="1">
       <c r="A165" s="3"/>
     </row>
-    <row r="166" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="166" spans="1:1" ht="16.5" customHeight="1">
       <c r="A166" s="3"/>
     </row>
-    <row r="167" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="167" spans="1:1" ht="16.5" customHeight="1">
       <c r="A167" s="3"/>
     </row>
   </sheetData>
-  <autoFilter ref="B1:E34" xr:uid="{00000000-0009-0000-0000-000001000000}"/>
+  <autoFilter ref="B1:E34"/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -2250,25 +2244,25 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:A14"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultRowHeight="13.5"/>
   <cols>
     <col min="1" max="1" width="55.5546875" style="1" customWidth="1"/>
     <col min="2" max="2" width="44.21875" style="1" customWidth="1"/>
     <col min="3" max="16384" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:1">
       <c r="A1" s="10"/>
     </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:1">
       <c r="A8" s="10"/>
     </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:1">
       <c r="A14" s="10"/>
     </row>
   </sheetData>
@@ -2279,14 +2273,14 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E165"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultRowHeight="13.5"/>
   <cols>
     <col min="1" max="1" width="2.77734375" style="9" customWidth="1"/>
     <col min="2" max="2" width="43.6640625" style="1" customWidth="1"/>
@@ -2296,7 +2290,7 @@
     <col min="6" max="16384" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:5">
       <c r="A1" s="7"/>
       <c r="B1" s="5" t="s">
         <v>8</v>
@@ -2311,496 +2305,496 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:5">
       <c r="A2" s="3"/>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:5">
       <c r="A3" s="8"/>
     </row>
-    <row r="4" spans="1:5" ht="36.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:5" ht="36.75" customHeight="1">
       <c r="A4" s="3"/>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:5">
       <c r="A5" s="8"/>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:5">
       <c r="A6" s="3"/>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:5">
       <c r="A7" s="3"/>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:5">
       <c r="A8" s="3"/>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:5">
       <c r="A9" s="3"/>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:5">
       <c r="A10" s="3"/>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:5">
       <c r="A11" s="8"/>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:5">
       <c r="A12" s="3"/>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:5">
       <c r="A13" s="3"/>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:5">
       <c r="A14" s="3"/>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:5">
       <c r="A15" s="3"/>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:5">
       <c r="A16" s="3"/>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:1">
       <c r="A17" s="8"/>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:1">
       <c r="A18" s="3"/>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:1">
       <c r="A19" s="3"/>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:1">
       <c r="A20" s="3"/>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:1">
       <c r="A21" s="3"/>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:1">
       <c r="A22" s="3"/>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:1">
       <c r="A23" s="8"/>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="24" spans="1:1">
       <c r="A24" s="3"/>
     </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="25" spans="1:1">
       <c r="A25" s="3"/>
     </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="26" spans="1:1">
       <c r="A26" s="3"/>
     </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="27" spans="1:1">
       <c r="A27" s="3"/>
     </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="28" spans="1:1">
       <c r="A28" s="3"/>
     </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="29" spans="1:1">
       <c r="A29" s="8"/>
     </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="30" spans="1:1">
       <c r="A30" s="8"/>
     </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="31" spans="1:1">
       <c r="A31" s="3"/>
     </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="32" spans="1:1">
       <c r="A32" s="3"/>
     </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="33" spans="1:1">
       <c r="A33" s="3"/>
     </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="34" spans="1:1">
       <c r="A34" s="3"/>
     </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="35" spans="1:1">
       <c r="A35" s="8"/>
     </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="36" spans="1:1">
       <c r="A36" s="8"/>
     </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="37" spans="1:1">
       <c r="A37" s="8"/>
     </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="38" spans="1:1">
       <c r="A38" s="8"/>
     </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="39" spans="1:1">
       <c r="A39" s="8"/>
     </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="40" spans="1:1">
       <c r="A40" s="8"/>
     </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="41" spans="1:1">
       <c r="A41" s="8"/>
     </row>
-    <row r="42" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="42" spans="1:1">
       <c r="A42" s="8"/>
     </row>
-    <row r="43" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="43" spans="1:1">
       <c r="A43" s="8"/>
     </row>
-    <row r="44" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="44" spans="1:1">
       <c r="A44" s="8"/>
     </row>
-    <row r="45" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="45" spans="1:1">
       <c r="A45" s="8"/>
     </row>
-    <row r="46" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="46" spans="1:1">
       <c r="A46" s="8"/>
     </row>
-    <row r="47" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="47" spans="1:1">
       <c r="A47" s="8"/>
     </row>
-    <row r="48" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="48" spans="1:1">
       <c r="A48" s="8"/>
     </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="49" spans="1:1">
       <c r="A49" s="8"/>
     </row>
-    <row r="50" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="50" spans="1:1">
       <c r="A50" s="8"/>
     </row>
-    <row r="51" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="51" spans="1:1">
       <c r="A51" s="8"/>
     </row>
-    <row r="52" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="52" spans="1:1">
       <c r="A52" s="8"/>
     </row>
-    <row r="53" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="53" spans="1:1">
       <c r="A53" s="8"/>
     </row>
-    <row r="54" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="54" spans="1:1">
       <c r="A54" s="8"/>
     </row>
-    <row r="55" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="55" spans="1:1">
       <c r="A55" s="8"/>
     </row>
-    <row r="56" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="56" spans="1:1">
       <c r="A56" s="8"/>
     </row>
-    <row r="57" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="57" spans="1:1">
       <c r="A57" s="8"/>
     </row>
-    <row r="58" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="58" spans="1:1">
       <c r="A58" s="8"/>
     </row>
-    <row r="59" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="59" spans="1:1">
       <c r="A59" s="8"/>
     </row>
-    <row r="60" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="60" spans="1:1">
       <c r="A60" s="8"/>
     </row>
-    <row r="61" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="61" spans="1:1">
       <c r="A61" s="8"/>
     </row>
-    <row r="62" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="62" spans="1:1">
       <c r="A62" s="8"/>
     </row>
-    <row r="63" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="63" spans="1:1">
       <c r="A63" s="8"/>
     </row>
-    <row r="64" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="64" spans="1:1">
       <c r="A64" s="8"/>
     </row>
-    <row r="65" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="65" spans="1:1">
       <c r="A65" s="8"/>
     </row>
-    <row r="66" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="66" spans="1:1">
       <c r="A66" s="8"/>
     </row>
-    <row r="67" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="67" spans="1:1">
       <c r="A67" s="8"/>
     </row>
-    <row r="68" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="68" spans="1:1">
       <c r="A68" s="8"/>
     </row>
-    <row r="69" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="69" spans="1:1">
       <c r="A69" s="8"/>
     </row>
-    <row r="70" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="70" spans="1:1">
       <c r="A70" s="8"/>
     </row>
-    <row r="71" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="71" spans="1:1">
       <c r="A71" s="8"/>
     </row>
-    <row r="72" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="72" spans="1:1">
       <c r="A72" s="8"/>
     </row>
-    <row r="73" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="73" spans="1:1">
       <c r="A73" s="8"/>
     </row>
-    <row r="74" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="74" spans="1:1">
       <c r="A74" s="8"/>
     </row>
-    <row r="75" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="75" spans="1:1">
       <c r="A75" s="8"/>
     </row>
-    <row r="76" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="76" spans="1:1">
       <c r="A76" s="8"/>
     </row>
-    <row r="77" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="77" spans="1:1">
       <c r="A77" s="8"/>
     </row>
-    <row r="78" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="78" spans="1:1">
       <c r="A78" s="8"/>
     </row>
-    <row r="79" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="79" spans="1:1">
       <c r="A79" s="8"/>
     </row>
-    <row r="80" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="80" spans="1:1">
       <c r="A80" s="8"/>
     </row>
-    <row r="81" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="81" spans="1:1">
       <c r="A81" s="8"/>
     </row>
-    <row r="82" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="82" spans="1:1">
       <c r="A82" s="8"/>
     </row>
-    <row r="83" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="83" spans="1:1">
       <c r="A83" s="8"/>
     </row>
-    <row r="84" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="84" spans="1:1">
       <c r="A84" s="8"/>
     </row>
-    <row r="85" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="85" spans="1:1">
       <c r="A85" s="8"/>
     </row>
-    <row r="86" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="86" spans="1:1">
       <c r="A86" s="8"/>
     </row>
-    <row r="87" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="87" spans="1:1">
       <c r="A87" s="8"/>
     </row>
-    <row r="88" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="88" spans="1:1">
       <c r="A88" s="8"/>
     </row>
-    <row r="89" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="89" spans="1:1">
       <c r="A89" s="8"/>
     </row>
-    <row r="90" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="90" spans="1:1">
       <c r="A90" s="8"/>
     </row>
-    <row r="91" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="91" spans="1:1">
       <c r="A91" s="8"/>
     </row>
-    <row r="92" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="92" spans="1:1">
       <c r="A92" s="8"/>
     </row>
-    <row r="93" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="93" spans="1:1">
       <c r="A93" s="8"/>
     </row>
-    <row r="94" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="94" spans="1:1">
       <c r="A94" s="8"/>
     </row>
-    <row r="95" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="95" spans="1:1">
       <c r="A95" s="8"/>
     </row>
-    <row r="96" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="96" spans="1:1">
       <c r="A96" s="8"/>
     </row>
-    <row r="97" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="97" spans="1:1">
       <c r="A97" s="8"/>
     </row>
-    <row r="98" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="98" spans="1:1">
       <c r="A98" s="8"/>
     </row>
-    <row r="99" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="99" spans="1:1">
       <c r="A99" s="8"/>
     </row>
-    <row r="100" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="100" spans="1:1">
       <c r="A100" s="8"/>
     </row>
-    <row r="101" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="101" spans="1:1">
       <c r="A101" s="8"/>
     </row>
-    <row r="102" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="102" spans="1:1">
       <c r="A102" s="8"/>
     </row>
-    <row r="103" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="103" spans="1:1">
       <c r="A103" s="8"/>
     </row>
-    <row r="104" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="104" spans="1:1">
       <c r="A104" s="8"/>
     </row>
-    <row r="105" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="105" spans="1:1">
       <c r="A105" s="8"/>
     </row>
-    <row r="106" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="106" spans="1:1">
       <c r="A106" s="8"/>
     </row>
-    <row r="107" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="107" spans="1:1">
       <c r="A107" s="8"/>
     </row>
-    <row r="108" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="108" spans="1:1">
       <c r="A108" s="8"/>
     </row>
-    <row r="109" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="109" spans="1:1">
       <c r="A109" s="8"/>
     </row>
-    <row r="110" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="110" spans="1:1">
       <c r="A110" s="8"/>
     </row>
-    <row r="111" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="111" spans="1:1">
       <c r="A111" s="8"/>
     </row>
-    <row r="112" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="112" spans="1:1">
       <c r="A112" s="8"/>
     </row>
-    <row r="113" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="113" spans="1:1">
       <c r="A113" s="8"/>
     </row>
-    <row r="114" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="114" spans="1:1">
       <c r="A114" s="8"/>
     </row>
-    <row r="115" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="115" spans="1:1">
       <c r="A115" s="8"/>
     </row>
-    <row r="116" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="116" spans="1:1">
       <c r="A116" s="8"/>
     </row>
-    <row r="117" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="117" spans="1:1">
       <c r="A117" s="8"/>
     </row>
-    <row r="118" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="118" spans="1:1">
       <c r="A118" s="8"/>
     </row>
-    <row r="119" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="119" spans="1:1">
       <c r="A119" s="8"/>
     </row>
-    <row r="120" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="120" spans="1:1">
       <c r="A120" s="8"/>
     </row>
-    <row r="121" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="121" spans="1:1">
       <c r="A121" s="8"/>
     </row>
-    <row r="122" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="122" spans="1:1">
       <c r="A122" s="8"/>
     </row>
-    <row r="123" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="123" spans="1:1">
       <c r="A123" s="8"/>
     </row>
-    <row r="124" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="124" spans="1:1">
       <c r="A124" s="8"/>
     </row>
-    <row r="125" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="125" spans="1:1">
       <c r="A125" s="8"/>
     </row>
-    <row r="126" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="126" spans="1:1">
       <c r="A126" s="8"/>
     </row>
-    <row r="127" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="127" spans="1:1">
       <c r="A127" s="8"/>
     </row>
-    <row r="128" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="128" spans="1:1">
       <c r="A128" s="8"/>
     </row>
-    <row r="129" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="129" spans="1:1">
       <c r="A129" s="8"/>
     </row>
-    <row r="130" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="130" spans="1:1">
       <c r="A130" s="8"/>
     </row>
-    <row r="131" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="131" spans="1:1">
       <c r="A131" s="8"/>
     </row>
-    <row r="132" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="132" spans="1:1">
       <c r="A132" s="8"/>
     </row>
-    <row r="133" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="133" spans="1:1">
       <c r="A133" s="8"/>
     </row>
-    <row r="134" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="134" spans="1:1">
       <c r="A134" s="8"/>
     </row>
-    <row r="135" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="135" spans="1:1">
       <c r="A135" s="8"/>
     </row>
-    <row r="136" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="136" spans="1:1">
       <c r="A136" s="8"/>
     </row>
-    <row r="137" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="137" spans="1:1">
       <c r="A137" s="8"/>
     </row>
-    <row r="138" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="138" spans="1:1">
       <c r="A138" s="8"/>
     </row>
-    <row r="139" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="139" spans="1:1">
       <c r="A139" s="8"/>
     </row>
-    <row r="140" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="140" spans="1:1">
       <c r="A140" s="8"/>
     </row>
-    <row r="141" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="141" spans="1:1">
       <c r="A141" s="8"/>
     </row>
-    <row r="142" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="142" spans="1:1">
       <c r="A142" s="8"/>
     </row>
-    <row r="143" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="143" spans="1:1">
       <c r="A143" s="8"/>
     </row>
-    <row r="144" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="144" spans="1:1">
       <c r="A144" s="8"/>
     </row>
-    <row r="145" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="145" spans="1:1">
       <c r="A145" s="8"/>
     </row>
-    <row r="146" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="146" spans="1:1">
       <c r="A146" s="8"/>
     </row>
-    <row r="147" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="147" spans="1:1">
       <c r="A147" s="8"/>
     </row>
-    <row r="148" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="148" spans="1:1">
       <c r="A148" s="8"/>
     </row>
-    <row r="149" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="149" spans="1:1">
       <c r="A149" s="8"/>
     </row>
-    <row r="150" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="150" spans="1:1">
       <c r="A150" s="8"/>
     </row>
-    <row r="151" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="151" spans="1:1">
       <c r="A151" s="8"/>
     </row>
-    <row r="152" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="152" spans="1:1">
       <c r="A152" s="8"/>
     </row>
-    <row r="153" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="153" spans="1:1">
       <c r="A153" s="8"/>
     </row>
-    <row r="154" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="154" spans="1:1">
       <c r="A154" s="8"/>
     </row>
-    <row r="155" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="155" spans="1:1">
       <c r="A155" s="8"/>
     </row>
-    <row r="156" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="156" spans="1:1">
       <c r="A156" s="8"/>
     </row>
-    <row r="157" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="157" spans="1:1">
       <c r="A157" s="8"/>
     </row>
-    <row r="158" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="158" spans="1:1">
       <c r="A158" s="8"/>
     </row>
-    <row r="159" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="159" spans="1:1">
       <c r="A159" s="8"/>
     </row>
-    <row r="160" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="160" spans="1:1">
       <c r="A160" s="8"/>
     </row>
-    <row r="161" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="161" spans="1:1">
       <c r="A161" s="8"/>
     </row>
-    <row r="162" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="162" spans="1:1">
       <c r="A162" s="8"/>
     </row>
-    <row r="163" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="163" spans="1:1">
       <c r="A163" s="8"/>
     </row>
-    <row r="164" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="164" spans="1:1">
       <c r="A164" s="8"/>
     </row>
-    <row r="165" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="165" spans="1:1">
       <c r="A165" s="8"/>
     </row>
   </sheetData>
@@ -2811,14 +2805,14 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="H36" sqref="H36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultRowHeight="13.5"/>
   <sheetData/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Add lucide-react --- to be applied in design
</commit_message>
<xml_diff>
--- a/docs/tasks.xlsx
+++ b/docs/tasks.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28827"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\dev\git\web\plan-it\docs\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48E3687B-EAA6-4D9C-9398-D93EF775C6D4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20610" windowHeight="11640" tabRatio="438"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15390" tabRatio="438" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Requirements" sheetId="1" r:id="rId1"/>
@@ -17,7 +23,7 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Defects!$B$1:$E$34</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Requirements!$B$1:$F$69</definedName>
   </definedNames>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -35,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="25">
   <si>
     <t>Task</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -135,16 +141,20 @@
     <t>screenshots in readme.md</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
+  <si>
+    <t>add lucide-react, to be applied in design</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="42" formatCode="_-&quot;₩&quot;* #,##0_-;\-&quot;₩&quot;* #,##0_-;_-&quot;₩&quot;* &quot;-&quot;_-;_-@_-"/>
     <numFmt numFmtId="176" formatCode="yy&quot;-&quot;m&quot;-&quot;d;@"/>
   </numFmts>
-  <fonts count="3">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <name val="돋움"/>
@@ -274,7 +284,7 @@
         <xdr:cNvPr id="2" name="TextBox 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0400-000002000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -320,9 +330,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 테마">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -360,7 +370,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -394,6 +404,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -428,9 +439,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -603,14 +615,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F165"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5" customHeight="1"/>
+  <sheetFormatPr defaultRowHeight="16.5" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="2.77734375" style="9" customWidth="1"/>
     <col min="2" max="2" width="59.21875" style="1" customWidth="1"/>
@@ -621,7 +633,7 @@
     <col min="7" max="16384" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="27" customHeight="1">
+    <row r="1" spans="1:6" ht="27" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="7"/>
       <c r="B1" s="5" t="s">
         <v>0</v>
@@ -639,7 +651,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:6" customFormat="1" ht="16.5" customHeight="1">
+    <row r="2" spans="1:6" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="3"/>
       <c r="B2" s="13" t="s">
         <v>12</v>
@@ -656,7 +668,7 @@
       </c>
       <c r="F2" s="12"/>
     </row>
-    <row r="3" spans="1:6" ht="16.5" customHeight="1">
+    <row r="3" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="8"/>
       <c r="B3" s="13" t="s">
         <v>11</v>
@@ -669,7 +681,7 @@
         <v>45777</v>
       </c>
     </row>
-    <row r="4" spans="1:6" customFormat="1" ht="16.5" customHeight="1">
+    <row r="4" spans="1:6" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="3"/>
       <c r="B4" t="s">
         <v>13</v>
@@ -688,20 +700,26 @@
         <v>20</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="16.5" customHeight="1">
+    <row r="5" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="8"/>
       <c r="B5" s="1" t="s">
         <v>14</v>
       </c>
       <c r="C5" s="3" t="str">
         <f t="shared" si="0"/>
-        <v/>
+        <v>✓</v>
       </c>
       <c r="D5" s="16">
         <v>45777</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" customFormat="1" ht="16.5" customHeight="1">
+      <c r="E5" s="16">
+        <v>45832</v>
+      </c>
+      <c r="F5" s="12" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="3"/>
       <c r="B6" t="s">
         <v>17</v>
@@ -718,7 +736,7 @@
       </c>
       <c r="F6" s="12"/>
     </row>
-    <row r="7" spans="1:6" customFormat="1" ht="18" customHeight="1">
+    <row r="7" spans="1:6" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="3"/>
       <c r="B7" t="s">
         <v>18</v>
@@ -735,7 +753,7 @@
       </c>
       <c r="F7" s="12"/>
     </row>
-    <row r="8" spans="1:6" customFormat="1" ht="17.25" customHeight="1">
+    <row r="8" spans="1:6" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="3"/>
       <c r="B8" s="1" t="s">
         <v>19</v>
@@ -750,7 +768,7 @@
       <c r="E8" s="15"/>
       <c r="F8" s="12"/>
     </row>
-    <row r="9" spans="1:6" customFormat="1" ht="16.5" customHeight="1">
+    <row r="9" spans="1:6" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="3"/>
       <c r="B9" t="s">
         <v>22</v>
@@ -767,7 +785,7 @@
       </c>
       <c r="F9" s="12"/>
     </row>
-    <row r="10" spans="1:6" customFormat="1" ht="16.5" customHeight="1">
+    <row r="10" spans="1:6" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="3"/>
       <c r="B10" t="s">
         <v>23</v>
@@ -784,14 +802,14 @@
       </c>
       <c r="F10" s="12"/>
     </row>
-    <row r="11" spans="1:6" ht="16.5" customHeight="1">
+    <row r="11" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A11" s="8"/>
       <c r="C11" s="3" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
-    <row r="12" spans="1:6" customFormat="1" ht="16.5" customHeight="1">
+    <row r="12" spans="1:6" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A12" s="3"/>
       <c r="C12" s="3" t="str">
         <f t="shared" si="0"/>
@@ -801,7 +819,7 @@
       <c r="E12" s="15"/>
       <c r="F12" s="12"/>
     </row>
-    <row r="13" spans="1:6" customFormat="1" ht="20.25" customHeight="1">
+    <row r="13" spans="1:6" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A13" s="3"/>
       <c r="C13" s="3" t="str">
         <f t="shared" si="0"/>
@@ -811,7 +829,7 @@
       <c r="E13" s="15"/>
       <c r="F13" s="12"/>
     </row>
-    <row r="14" spans="1:6" customFormat="1" ht="20.25" customHeight="1">
+    <row r="14" spans="1:6" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A14" s="3"/>
       <c r="C14" s="3" t="str">
         <f t="shared" si="0"/>
@@ -821,7 +839,7 @@
       <c r="E14" s="15"/>
       <c r="F14" s="12"/>
     </row>
-    <row r="15" spans="1:6" customFormat="1" ht="16.5" customHeight="1">
+    <row r="15" spans="1:6" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A15" s="3"/>
       <c r="C15" s="3" t="str">
         <f t="shared" si="0"/>
@@ -831,7 +849,7 @@
       <c r="E15" s="15"/>
       <c r="F15" s="12"/>
     </row>
-    <row r="16" spans="1:6" customFormat="1" ht="16.5" customHeight="1">
+    <row r="16" spans="1:6" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A16" s="3"/>
       <c r="C16" s="3" t="str">
         <f t="shared" si="0"/>
@@ -841,14 +859,14 @@
       <c r="E16" s="15"/>
       <c r="F16" s="12"/>
     </row>
-    <row r="17" spans="1:6" ht="16.5" customHeight="1">
+    <row r="17" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A17" s="8"/>
       <c r="C17" s="3" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
-    <row r="18" spans="1:6" customFormat="1" ht="16.5" customHeight="1">
+    <row r="18" spans="1:6" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A18" s="3"/>
       <c r="C18" s="3" t="str">
         <f t="shared" si="0"/>
@@ -858,7 +876,7 @@
       <c r="E18" s="15"/>
       <c r="F18" s="12"/>
     </row>
-    <row r="19" spans="1:6" customFormat="1" ht="16.5" customHeight="1">
+    <row r="19" spans="1:6" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A19" s="3"/>
       <c r="C19" s="3" t="str">
         <f t="shared" si="0"/>
@@ -868,7 +886,7 @@
       <c r="E19" s="15"/>
       <c r="F19" s="12"/>
     </row>
-    <row r="20" spans="1:6" customFormat="1" ht="16.5" customHeight="1">
+    <row r="20" spans="1:6" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A20" s="3"/>
       <c r="C20" s="3" t="str">
         <f t="shared" si="0"/>
@@ -878,7 +896,7 @@
       <c r="E20" s="15"/>
       <c r="F20" s="12"/>
     </row>
-    <row r="21" spans="1:6" customFormat="1" ht="16.5" customHeight="1">
+    <row r="21" spans="1:6" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A21" s="3"/>
       <c r="C21" s="3" t="str">
         <f t="shared" si="0"/>
@@ -888,7 +906,7 @@
       <c r="E21" s="15"/>
       <c r="F21" s="12"/>
     </row>
-    <row r="22" spans="1:6" customFormat="1" ht="16.5" customHeight="1">
+    <row r="22" spans="1:6" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A22" s="3"/>
       <c r="C22" s="3" t="str">
         <f t="shared" si="0"/>
@@ -898,14 +916,14 @@
       <c r="E22" s="15"/>
       <c r="F22" s="12"/>
     </row>
-    <row r="23" spans="1:6" ht="16.5" customHeight="1">
+    <row r="23" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A23" s="8"/>
       <c r="C23" s="3" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
-    <row r="24" spans="1:6" customFormat="1" ht="16.5" customHeight="1">
+    <row r="24" spans="1:6" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A24" s="3"/>
       <c r="C24" s="3" t="str">
         <f t="shared" si="0"/>
@@ -915,7 +933,7 @@
       <c r="E24" s="15"/>
       <c r="F24" s="12"/>
     </row>
-    <row r="25" spans="1:6" customFormat="1" ht="16.5" customHeight="1">
+    <row r="25" spans="1:6" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A25" s="3"/>
       <c r="C25" s="3" t="str">
         <f t="shared" si="0"/>
@@ -925,7 +943,7 @@
       <c r="E25" s="15"/>
       <c r="F25" s="12"/>
     </row>
-    <row r="26" spans="1:6" customFormat="1" ht="16.5" customHeight="1">
+    <row r="26" spans="1:6" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A26" s="3"/>
       <c r="C26" s="3" t="str">
         <f t="shared" si="0"/>
@@ -935,7 +953,7 @@
       <c r="E26" s="15"/>
       <c r="F26" s="12"/>
     </row>
-    <row r="27" spans="1:6" customFormat="1" ht="16.5" customHeight="1">
+    <row r="27" spans="1:6" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A27" s="3"/>
       <c r="C27" s="3" t="str">
         <f t="shared" si="0"/>
@@ -945,7 +963,7 @@
       <c r="E27" s="15"/>
       <c r="F27" s="12"/>
     </row>
-    <row r="28" spans="1:6" customFormat="1" ht="16.5" customHeight="1">
+    <row r="28" spans="1:6" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A28" s="3"/>
       <c r="C28" s="3" t="str">
         <f t="shared" si="0"/>
@@ -955,21 +973,21 @@
       <c r="E28" s="15"/>
       <c r="F28" s="12"/>
     </row>
-    <row r="29" spans="1:6" ht="16.5" customHeight="1">
+    <row r="29" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A29" s="8"/>
       <c r="C29" s="3" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
-    <row r="30" spans="1:6" ht="16.5" customHeight="1">
+    <row r="30" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A30" s="8"/>
       <c r="C30" s="3" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
-    <row r="31" spans="1:6" customFormat="1" ht="16.5" customHeight="1">
+    <row r="31" spans="1:6" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A31" s="3"/>
       <c r="C31" s="3" t="str">
         <f t="shared" si="0"/>
@@ -979,7 +997,7 @@
       <c r="E31" s="15"/>
       <c r="F31" s="12"/>
     </row>
-    <row r="32" spans="1:6" customFormat="1" ht="16.5" customHeight="1">
+    <row r="32" spans="1:6" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A32" s="3"/>
       <c r="C32" s="3" t="str">
         <f t="shared" si="0"/>
@@ -989,7 +1007,7 @@
       <c r="E32" s="15"/>
       <c r="F32" s="12"/>
     </row>
-    <row r="33" spans="1:6" customFormat="1" ht="16.5" customHeight="1">
+    <row r="33" spans="1:6" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A33" s="3"/>
       <c r="C33" s="3" t="str">
         <f t="shared" si="0"/>
@@ -999,7 +1017,7 @@
       <c r="E33" s="15"/>
       <c r="F33" s="12"/>
     </row>
-    <row r="34" spans="1:6" customFormat="1" ht="53.25" customHeight="1">
+    <row r="34" spans="1:6" customFormat="1" ht="53.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A34" s="3"/>
       <c r="C34" s="3" t="str">
         <f t="shared" si="0"/>
@@ -1009,401 +1027,401 @@
       <c r="E34" s="15"/>
       <c r="F34" s="12"/>
     </row>
-    <row r="35" spans="1:6" ht="48.75" customHeight="1">
+    <row r="35" spans="1:6" ht="48.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A35" s="8"/>
     </row>
-    <row r="36" spans="1:6" ht="16.5" customHeight="1">
+    <row r="36" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A36" s="8"/>
     </row>
-    <row r="37" spans="1:6" ht="16.5" customHeight="1">
+    <row r="37" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A37" s="8"/>
     </row>
-    <row r="38" spans="1:6" ht="16.5" customHeight="1">
+    <row r="38" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A38" s="8"/>
     </row>
-    <row r="39" spans="1:6" ht="16.5" customHeight="1">
+    <row r="39" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A39" s="8"/>
     </row>
-    <row r="40" spans="1:6" ht="16.5" customHeight="1">
+    <row r="40" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A40" s="8"/>
     </row>
-    <row r="41" spans="1:6" ht="37.5" customHeight="1">
+    <row r="41" spans="1:6" ht="37.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A41" s="8"/>
     </row>
-    <row r="42" spans="1:6" ht="16.5" customHeight="1">
+    <row r="42" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A42" s="8"/>
     </row>
-    <row r="43" spans="1:6" ht="16.5" customHeight="1">
+    <row r="43" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A43" s="8"/>
     </row>
-    <row r="44" spans="1:6" ht="16.5" customHeight="1">
+    <row r="44" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A44" s="8"/>
     </row>
-    <row r="45" spans="1:6" ht="16.5" customHeight="1">
+    <row r="45" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A45" s="8"/>
     </row>
-    <row r="46" spans="1:6" ht="16.5" customHeight="1">
+    <row r="46" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A46" s="8"/>
     </row>
-    <row r="47" spans="1:6" ht="16.5" customHeight="1">
+    <row r="47" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A47" s="8"/>
     </row>
-    <row r="48" spans="1:6" ht="16.5" customHeight="1">
+    <row r="48" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A48" s="8"/>
     </row>
-    <row r="49" spans="1:1" ht="16.5" customHeight="1">
+    <row r="49" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A49" s="8"/>
     </row>
-    <row r="50" spans="1:1" ht="16.5" customHeight="1">
+    <row r="50" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A50" s="8"/>
     </row>
-    <row r="51" spans="1:1" ht="16.5" customHeight="1">
+    <row r="51" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A51" s="8"/>
     </row>
-    <row r="52" spans="1:1" ht="16.5" customHeight="1">
+    <row r="52" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A52" s="8"/>
     </row>
-    <row r="53" spans="1:1" ht="16.5" customHeight="1">
+    <row r="53" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A53" s="8"/>
     </row>
-    <row r="54" spans="1:1" ht="16.5" customHeight="1">
+    <row r="54" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A54" s="8"/>
     </row>
-    <row r="55" spans="1:1" ht="16.5" customHeight="1">
+    <row r="55" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A55" s="8"/>
     </row>
-    <row r="56" spans="1:1" ht="16.5" customHeight="1">
+    <row r="56" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A56" s="8"/>
     </row>
-    <row r="57" spans="1:1" ht="32.25" customHeight="1">
+    <row r="57" spans="1:1" ht="32.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A57" s="8"/>
     </row>
-    <row r="58" spans="1:1" ht="49.5" customHeight="1">
+    <row r="58" spans="1:1" ht="49.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A58" s="8"/>
     </row>
-    <row r="59" spans="1:1" ht="16.5" customHeight="1">
+    <row r="59" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A59" s="8"/>
     </row>
-    <row r="60" spans="1:1" ht="16.5" customHeight="1">
+    <row r="60" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A60" s="8"/>
     </row>
-    <row r="61" spans="1:1" ht="16.5" customHeight="1">
+    <row r="61" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A61" s="8"/>
     </row>
-    <row r="62" spans="1:1" ht="16.5" customHeight="1">
+    <row r="62" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A62" s="8"/>
     </row>
-    <row r="63" spans="1:1" ht="16.5" customHeight="1">
+    <row r="63" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A63" s="8"/>
     </row>
-    <row r="64" spans="1:1" ht="16.5" customHeight="1">
+    <row r="64" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A64" s="8"/>
     </row>
-    <row r="65" spans="1:1" ht="16.5" customHeight="1">
+    <row r="65" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A65" s="8"/>
     </row>
-    <row r="66" spans="1:1" ht="16.5" customHeight="1">
+    <row r="66" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A66" s="8"/>
     </row>
-    <row r="67" spans="1:1" ht="16.5" customHeight="1">
+    <row r="67" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A67" s="8"/>
     </row>
-    <row r="68" spans="1:1" ht="16.5" customHeight="1">
+    <row r="68" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A68" s="8"/>
     </row>
-    <row r="69" spans="1:1" ht="27.75" customHeight="1">
+    <row r="69" spans="1:1" ht="27.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A69" s="8"/>
     </row>
-    <row r="70" spans="1:1" ht="16.5" customHeight="1">
+    <row r="70" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A70" s="8"/>
     </row>
-    <row r="71" spans="1:1" ht="16.5" customHeight="1">
+    <row r="71" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A71" s="8"/>
     </row>
-    <row r="72" spans="1:1" ht="16.5" customHeight="1">
+    <row r="72" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A72" s="8"/>
     </row>
-    <row r="73" spans="1:1" ht="16.5" customHeight="1">
+    <row r="73" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A73" s="8"/>
     </row>
-    <row r="74" spans="1:1" ht="16.5" customHeight="1">
+    <row r="74" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A74" s="8"/>
     </row>
-    <row r="75" spans="1:1" ht="16.5" customHeight="1">
+    <row r="75" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A75" s="8"/>
     </row>
-    <row r="76" spans="1:1" ht="16.5" customHeight="1">
+    <row r="76" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A76" s="8"/>
     </row>
-    <row r="77" spans="1:1" ht="16.5" customHeight="1">
+    <row r="77" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A77" s="8"/>
     </row>
-    <row r="78" spans="1:1" ht="16.5" customHeight="1">
+    <row r="78" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A78" s="8"/>
     </row>
-    <row r="79" spans="1:1" ht="16.5" customHeight="1">
+    <row r="79" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A79" s="8"/>
     </row>
-    <row r="80" spans="1:1" ht="16.5" customHeight="1">
+    <row r="80" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A80" s="8"/>
     </row>
-    <row r="81" spans="1:1" ht="16.5" customHeight="1">
+    <row r="81" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A81" s="8"/>
     </row>
-    <row r="82" spans="1:1" ht="16.5" customHeight="1">
+    <row r="82" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A82" s="8"/>
     </row>
-    <row r="83" spans="1:1" ht="16.5" customHeight="1">
+    <row r="83" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A83" s="8"/>
     </row>
-    <row r="84" spans="1:1" ht="16.5" customHeight="1">
+    <row r="84" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A84" s="8"/>
     </row>
-    <row r="85" spans="1:1" ht="16.5" customHeight="1">
+    <row r="85" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A85" s="8"/>
     </row>
-    <row r="86" spans="1:1" ht="16.5" customHeight="1">
+    <row r="86" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A86" s="8"/>
     </row>
-    <row r="87" spans="1:1" ht="16.5" customHeight="1">
+    <row r="87" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A87" s="8"/>
     </row>
-    <row r="88" spans="1:1" ht="16.5" customHeight="1">
+    <row r="88" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A88" s="8"/>
     </row>
-    <row r="89" spans="1:1" ht="16.5" customHeight="1">
+    <row r="89" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A89" s="8"/>
     </row>
-    <row r="90" spans="1:1" ht="16.5" customHeight="1">
+    <row r="90" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A90" s="8"/>
     </row>
-    <row r="91" spans="1:1" ht="16.5" customHeight="1">
+    <row r="91" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A91" s="8"/>
     </row>
-    <row r="92" spans="1:1" ht="16.5" customHeight="1">
+    <row r="92" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A92" s="8"/>
     </row>
-    <row r="93" spans="1:1" ht="16.5" customHeight="1">
+    <row r="93" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A93" s="8"/>
     </row>
-    <row r="94" spans="1:1" ht="16.5" customHeight="1">
+    <row r="94" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A94" s="8"/>
     </row>
-    <row r="95" spans="1:1" ht="16.5" customHeight="1">
+    <row r="95" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A95" s="8"/>
     </row>
-    <row r="96" spans="1:1" ht="16.5" customHeight="1">
+    <row r="96" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A96" s="8"/>
     </row>
-    <row r="97" spans="1:1" ht="16.5" customHeight="1">
+    <row r="97" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A97" s="8"/>
     </row>
-    <row r="98" spans="1:1" ht="16.5" customHeight="1">
+    <row r="98" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A98" s="8"/>
     </row>
-    <row r="99" spans="1:1" ht="16.5" customHeight="1">
+    <row r="99" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A99" s="8"/>
     </row>
-    <row r="100" spans="1:1" ht="16.5" customHeight="1">
+    <row r="100" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A100" s="8"/>
     </row>
-    <row r="101" spans="1:1" ht="16.5" customHeight="1">
+    <row r="101" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A101" s="8"/>
     </row>
-    <row r="102" spans="1:1" ht="16.5" customHeight="1">
+    <row r="102" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A102" s="8"/>
     </row>
-    <row r="103" spans="1:1" ht="16.5" customHeight="1">
+    <row r="103" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A103" s="8"/>
     </row>
-    <row r="104" spans="1:1" ht="16.5" customHeight="1">
+    <row r="104" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A104" s="8"/>
     </row>
-    <row r="105" spans="1:1" ht="16.5" customHeight="1">
+    <row r="105" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A105" s="8"/>
     </row>
-    <row r="106" spans="1:1" ht="16.5" customHeight="1">
+    <row r="106" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A106" s="8"/>
     </row>
-    <row r="107" spans="1:1" ht="16.5" customHeight="1">
+    <row r="107" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A107" s="8"/>
     </row>
-    <row r="108" spans="1:1" ht="16.5" customHeight="1">
+    <row r="108" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A108" s="8"/>
     </row>
-    <row r="109" spans="1:1" ht="16.5" customHeight="1">
+    <row r="109" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A109" s="8"/>
     </row>
-    <row r="110" spans="1:1" ht="16.5" customHeight="1">
+    <row r="110" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A110" s="8"/>
     </row>
-    <row r="111" spans="1:1" ht="16.5" customHeight="1">
+    <row r="111" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A111" s="8"/>
     </row>
-    <row r="112" spans="1:1" ht="16.5" customHeight="1">
+    <row r="112" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A112" s="8"/>
     </row>
-    <row r="113" spans="1:1" ht="16.5" customHeight="1">
+    <row r="113" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A113" s="8"/>
     </row>
-    <row r="114" spans="1:1" ht="16.5" customHeight="1">
+    <row r="114" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A114" s="8"/>
     </row>
-    <row r="115" spans="1:1" ht="16.5" customHeight="1">
+    <row r="115" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A115" s="8"/>
     </row>
-    <row r="116" spans="1:1" ht="16.5" customHeight="1">
+    <row r="116" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A116" s="8"/>
     </row>
-    <row r="117" spans="1:1" ht="16.5" customHeight="1">
+    <row r="117" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A117" s="8"/>
     </row>
-    <row r="118" spans="1:1" ht="16.5" customHeight="1">
+    <row r="118" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A118" s="8"/>
     </row>
-    <row r="119" spans="1:1" ht="16.5" customHeight="1">
+    <row r="119" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A119" s="8"/>
     </row>
-    <row r="120" spans="1:1" ht="16.5" customHeight="1">
+    <row r="120" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A120" s="8"/>
     </row>
-    <row r="121" spans="1:1" ht="16.5" customHeight="1">
+    <row r="121" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A121" s="8"/>
     </row>
-    <row r="122" spans="1:1" ht="16.5" customHeight="1">
+    <row r="122" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A122" s="8"/>
     </row>
-    <row r="123" spans="1:1" ht="16.5" customHeight="1">
+    <row r="123" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A123" s="8"/>
     </row>
-    <row r="124" spans="1:1" ht="16.5" customHeight="1">
+    <row r="124" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A124" s="8"/>
     </row>
-    <row r="125" spans="1:1" ht="16.5" customHeight="1">
+    <row r="125" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A125" s="8"/>
     </row>
-    <row r="126" spans="1:1" ht="16.5" customHeight="1">
+    <row r="126" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A126" s="8"/>
     </row>
-    <row r="127" spans="1:1" ht="16.5" customHeight="1">
+    <row r="127" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A127" s="8"/>
     </row>
-    <row r="128" spans="1:1" ht="16.5" customHeight="1">
+    <row r="128" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A128" s="8"/>
     </row>
-    <row r="129" spans="1:1" ht="16.5" customHeight="1">
+    <row r="129" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A129" s="8"/>
     </row>
-    <row r="130" spans="1:1" ht="16.5" customHeight="1">
+    <row r="130" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A130" s="8"/>
     </row>
-    <row r="131" spans="1:1" ht="16.5" customHeight="1">
+    <row r="131" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A131" s="8"/>
     </row>
-    <row r="132" spans="1:1" ht="16.5" customHeight="1">
+    <row r="132" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A132" s="8"/>
     </row>
-    <row r="133" spans="1:1" ht="16.5" customHeight="1">
+    <row r="133" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A133" s="8"/>
     </row>
-    <row r="134" spans="1:1" ht="16.5" customHeight="1">
+    <row r="134" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A134" s="8"/>
     </row>
-    <row r="135" spans="1:1" ht="16.5" customHeight="1">
+    <row r="135" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A135" s="8"/>
     </row>
-    <row r="136" spans="1:1" ht="16.5" customHeight="1">
+    <row r="136" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A136" s="8"/>
     </row>
-    <row r="137" spans="1:1" ht="16.5" customHeight="1">
+    <row r="137" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A137" s="8"/>
     </row>
-    <row r="138" spans="1:1" ht="16.5" customHeight="1">
+    <row r="138" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A138" s="8"/>
     </row>
-    <row r="139" spans="1:1" ht="16.5" customHeight="1">
+    <row r="139" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A139" s="8"/>
     </row>
-    <row r="140" spans="1:1" ht="16.5" customHeight="1">
+    <row r="140" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A140" s="8"/>
     </row>
-    <row r="141" spans="1:1" ht="16.5" customHeight="1">
+    <row r="141" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A141" s="8"/>
     </row>
-    <row r="142" spans="1:1" ht="16.5" customHeight="1">
+    <row r="142" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A142" s="8"/>
     </row>
-    <row r="143" spans="1:1" ht="16.5" customHeight="1">
+    <row r="143" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A143" s="8"/>
     </row>
-    <row r="144" spans="1:1" ht="16.5" customHeight="1">
+    <row r="144" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A144" s="8"/>
     </row>
-    <row r="145" spans="1:1" ht="16.5" customHeight="1">
+    <row r="145" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A145" s="8"/>
     </row>
-    <row r="146" spans="1:1" ht="16.5" customHeight="1">
+    <row r="146" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A146" s="8"/>
     </row>
-    <row r="147" spans="1:1" ht="16.5" customHeight="1">
+    <row r="147" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A147" s="8"/>
     </row>
-    <row r="148" spans="1:1" ht="16.5" customHeight="1">
+    <row r="148" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A148" s="8"/>
     </row>
-    <row r="149" spans="1:1" ht="16.5" customHeight="1">
+    <row r="149" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A149" s="8"/>
     </row>
-    <row r="150" spans="1:1" ht="16.5" customHeight="1">
+    <row r="150" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A150" s="8"/>
     </row>
-    <row r="151" spans="1:1" ht="16.5" customHeight="1">
+    <row r="151" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A151" s="8"/>
     </row>
-    <row r="152" spans="1:1" ht="16.5" customHeight="1">
+    <row r="152" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A152" s="8"/>
     </row>
-    <row r="153" spans="1:1" ht="16.5" customHeight="1">
+    <row r="153" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A153" s="8"/>
     </row>
-    <row r="154" spans="1:1" ht="16.5" customHeight="1">
+    <row r="154" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A154" s="8"/>
     </row>
-    <row r="155" spans="1:1" ht="16.5" customHeight="1">
+    <row r="155" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A155" s="8"/>
     </row>
-    <row r="156" spans="1:1" ht="16.5" customHeight="1">
+    <row r="156" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A156" s="8"/>
     </row>
-    <row r="157" spans="1:1" ht="16.5" customHeight="1">
+    <row r="157" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A157" s="8"/>
     </row>
-    <row r="158" spans="1:1" ht="16.5" customHeight="1">
+    <row r="158" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A158" s="8"/>
     </row>
-    <row r="159" spans="1:1" ht="16.5" customHeight="1">
+    <row r="159" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A159" s="8"/>
     </row>
-    <row r="160" spans="1:1" ht="16.5" customHeight="1">
+    <row r="160" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A160" s="8"/>
     </row>
-    <row r="161" spans="1:1" ht="16.5" customHeight="1">
+    <row r="161" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A161" s="8"/>
     </row>
-    <row r="162" spans="1:1" ht="16.5" customHeight="1">
+    <row r="162" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A162" s="8"/>
     </row>
-    <row r="163" spans="1:1" ht="16.5" customHeight="1">
+    <row r="163" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A163" s="8"/>
     </row>
-    <row r="164" spans="1:1" ht="16.5" customHeight="1">
+    <row r="164" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A164" s="8"/>
     </row>
-    <row r="165" spans="1:1" ht="16.5" customHeight="1">
+    <row r="165" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A165" s="8"/>
     </row>
   </sheetData>
-  <autoFilter ref="B1:F69"/>
+  <autoFilter ref="B1:F69" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -1412,14 +1430,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:F167"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5" customHeight="1"/>
+  <sheetFormatPr defaultRowHeight="16.5" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="1.6640625" style="14" customWidth="1"/>
     <col min="2" max="2" width="59.21875" style="1" customWidth="1"/>
@@ -1429,7 +1447,7 @@
     <col min="6" max="6" width="50.21875" style="12" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="30.75" customHeight="1">
+    <row r="1" spans="1:6" ht="30.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="2"/>
       <c r="B1" s="5" t="s">
         <v>3</v>
@@ -1447,7 +1465,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="16.5" customHeight="1">
+    <row r="2" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="3"/>
       <c r="B2" t="s">
         <v>16</v>
@@ -1463,7 +1481,7 @@
         <v>45777</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="16.5" customHeight="1">
+    <row r="3" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="3"/>
       <c r="B3" s="17" t="s">
         <v>15</v>
@@ -1479,7 +1497,7 @@
         <v>45777</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="16.5" customHeight="1">
+    <row r="4" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="3"/>
       <c r="B4" t="s">
         <v>21</v>
@@ -1495,14 +1513,14 @@
         <v>45779</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="16.5" customHeight="1">
+    <row r="5" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="3"/>
       <c r="C5" s="3" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="33.75" customHeight="1">
+    <row r="6" spans="1:6" ht="33.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="3"/>
       <c r="B6"/>
       <c r="C6" s="3" t="str">
@@ -1512,7 +1530,7 @@
       <c r="D6" s="15"/>
       <c r="E6" s="15"/>
     </row>
-    <row r="7" spans="1:6" ht="16.5" customHeight="1">
+    <row r="7" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="3"/>
       <c r="B7"/>
       <c r="C7" s="3" t="str">
@@ -1522,7 +1540,7 @@
       <c r="D7" s="15"/>
       <c r="E7" s="15"/>
     </row>
-    <row r="8" spans="1:6" ht="16.5" customHeight="1">
+    <row r="8" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="3"/>
       <c r="C8" s="3" t="str">
         <f t="shared" si="0"/>
@@ -1531,7 +1549,7 @@
       <c r="D8" s="15"/>
       <c r="E8" s="15"/>
     </row>
-    <row r="9" spans="1:6" ht="13.5">
+    <row r="9" spans="1:6" ht="13.5" x14ac:dyDescent="0.15">
       <c r="A9" s="3"/>
       <c r="B9"/>
       <c r="C9" s="3" t="str">
@@ -1541,7 +1559,7 @@
       <c r="D9" s="15"/>
       <c r="E9" s="15"/>
     </row>
-    <row r="10" spans="1:6" ht="16.5" customHeight="1">
+    <row r="10" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="3"/>
       <c r="B10"/>
       <c r="C10" s="3" t="str">
@@ -1551,14 +1569,14 @@
       <c r="D10" s="15"/>
       <c r="E10" s="15"/>
     </row>
-    <row r="11" spans="1:6" ht="36.75" customHeight="1">
+    <row r="11" spans="1:6" ht="36.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A11" s="3"/>
       <c r="C11" s="3" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
-    <row r="12" spans="1:6" ht="32.25" customHeight="1">
+    <row r="12" spans="1:6" ht="32.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A12" s="3"/>
       <c r="B12"/>
       <c r="C12" s="3" t="str">
@@ -1568,7 +1586,7 @@
       <c r="D12" s="15"/>
       <c r="E12" s="15"/>
     </row>
-    <row r="13" spans="1:6" ht="16.5" customHeight="1">
+    <row r="13" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A13" s="3"/>
       <c r="B13"/>
       <c r="C13" s="3" t="str">
@@ -1578,7 +1596,7 @@
       <c r="D13" s="15"/>
       <c r="E13" s="15"/>
     </row>
-    <row r="14" spans="1:6" ht="16.5" customHeight="1">
+    <row r="14" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A14" s="3"/>
       <c r="B14"/>
       <c r="C14" s="3" t="str">
@@ -1588,7 +1606,7 @@
       <c r="D14" s="15"/>
       <c r="E14" s="15"/>
     </row>
-    <row r="15" spans="1:6" ht="16.5" customHeight="1">
+    <row r="15" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A15" s="3"/>
       <c r="B15"/>
       <c r="C15" s="3" t="str">
@@ -1598,7 +1616,7 @@
       <c r="D15" s="15"/>
       <c r="E15" s="15"/>
     </row>
-    <row r="16" spans="1:6" ht="16.5" customHeight="1">
+    <row r="16" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A16" s="3"/>
       <c r="B16"/>
       <c r="C16" s="3" t="str">
@@ -1608,14 +1626,14 @@
       <c r="D16" s="15"/>
       <c r="E16" s="15"/>
     </row>
-    <row r="17" spans="1:5" ht="16.5" customHeight="1">
+    <row r="17" spans="1:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A17" s="3"/>
       <c r="C17" s="3" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
-    <row r="18" spans="1:5" ht="39" customHeight="1">
+    <row r="18" spans="1:5" ht="39" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A18" s="3"/>
       <c r="B18"/>
       <c r="C18" s="3" t="str">
@@ -1625,7 +1643,7 @@
       <c r="D18" s="15"/>
       <c r="E18" s="15"/>
     </row>
-    <row r="19" spans="1:5" ht="45.75" customHeight="1">
+    <row r="19" spans="1:5" ht="45.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A19" s="3"/>
       <c r="B19"/>
       <c r="C19" s="3" t="str">
@@ -1635,7 +1653,7 @@
       <c r="D19" s="15"/>
       <c r="E19" s="15"/>
     </row>
-    <row r="20" spans="1:5" ht="16.5" customHeight="1">
+    <row r="20" spans="1:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A20" s="3"/>
       <c r="B20"/>
       <c r="C20" s="3" t="str">
@@ -1645,7 +1663,7 @@
       <c r="D20" s="15"/>
       <c r="E20" s="15"/>
     </row>
-    <row r="21" spans="1:5" ht="16.5" customHeight="1">
+    <row r="21" spans="1:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A21" s="3"/>
       <c r="B21"/>
       <c r="C21" s="3" t="str">
@@ -1655,7 +1673,7 @@
       <c r="D21" s="15"/>
       <c r="E21" s="15"/>
     </row>
-    <row r="22" spans="1:5" ht="13.5">
+    <row r="22" spans="1:5" ht="13.5" x14ac:dyDescent="0.15">
       <c r="A22" s="3"/>
       <c r="B22"/>
       <c r="C22" s="3" t="str">
@@ -1665,14 +1683,14 @@
       <c r="D22" s="15"/>
       <c r="E22" s="15"/>
     </row>
-    <row r="23" spans="1:5" ht="16.5" customHeight="1">
+    <row r="23" spans="1:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A23" s="3"/>
       <c r="C23" s="3" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
-    <row r="24" spans="1:5" ht="16.5" customHeight="1">
+    <row r="24" spans="1:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A24" s="3"/>
       <c r="B24"/>
       <c r="C24" s="3" t="str">
@@ -1682,7 +1700,7 @@
       <c r="D24" s="15"/>
       <c r="E24" s="15"/>
     </row>
-    <row r="25" spans="1:5" ht="16.5" customHeight="1">
+    <row r="25" spans="1:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A25" s="3"/>
       <c r="B25"/>
       <c r="C25" s="3" t="str">
@@ -1692,7 +1710,7 @@
       <c r="D25" s="15"/>
       <c r="E25" s="15"/>
     </row>
-    <row r="26" spans="1:5" ht="34.5" customHeight="1">
+    <row r="26" spans="1:5" ht="34.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A26" s="3"/>
       <c r="B26"/>
       <c r="C26" s="3" t="str">
@@ -1702,7 +1720,7 @@
       <c r="D26" s="15"/>
       <c r="E26" s="15"/>
     </row>
-    <row r="27" spans="1:5" ht="29.25" customHeight="1">
+    <row r="27" spans="1:5" ht="29.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A27" s="3"/>
       <c r="B27"/>
       <c r="C27" s="3" t="str">
@@ -1712,7 +1730,7 @@
       <c r="D27" s="15"/>
       <c r="E27" s="15"/>
     </row>
-    <row r="28" spans="1:5" ht="16.5" customHeight="1">
+    <row r="28" spans="1:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A28" s="3"/>
       <c r="B28"/>
       <c r="C28" s="3" t="str">
@@ -1722,21 +1740,21 @@
       <c r="D28" s="15"/>
       <c r="E28" s="15"/>
     </row>
-    <row r="29" spans="1:5" ht="16.5" customHeight="1">
+    <row r="29" spans="1:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A29" s="3"/>
       <c r="C29" s="3" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
-    <row r="30" spans="1:5" ht="36.75" customHeight="1">
+    <row r="30" spans="1:5" ht="36.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A30" s="3"/>
       <c r="C30" s="3" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
-    <row r="31" spans="1:5" ht="54.75" customHeight="1">
+    <row r="31" spans="1:5" ht="54.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A31" s="3"/>
       <c r="B31"/>
       <c r="C31" s="3" t="str">
@@ -1746,7 +1764,7 @@
       <c r="D31" s="15"/>
       <c r="E31" s="15"/>
     </row>
-    <row r="32" spans="1:5" ht="16.5" customHeight="1">
+    <row r="32" spans="1:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A32" s="3"/>
       <c r="B32"/>
       <c r="C32" s="3" t="str">
@@ -1756,7 +1774,7 @@
       <c r="D32" s="15"/>
       <c r="E32" s="15"/>
     </row>
-    <row r="33" spans="1:5" ht="16.5" customHeight="1">
+    <row r="33" spans="1:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A33" s="3"/>
       <c r="B33"/>
       <c r="C33" s="3" t="str">
@@ -1766,7 +1784,7 @@
       <c r="D33" s="15"/>
       <c r="E33" s="15"/>
     </row>
-    <row r="34" spans="1:5" ht="16.5" customHeight="1">
+    <row r="34" spans="1:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A34" s="3"/>
       <c r="B34"/>
       <c r="C34" s="3" t="str">
@@ -1776,467 +1794,467 @@
       <c r="D34" s="15"/>
       <c r="E34" s="15"/>
     </row>
-    <row r="35" spans="1:5" ht="34.5" customHeight="1">
+    <row r="35" spans="1:5" ht="34.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A35" s="3"/>
       <c r="C35" s="3" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
-    <row r="36" spans="1:5" ht="16.5" customHeight="1">
+    <row r="36" spans="1:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A36" s="3"/>
       <c r="C36" s="3" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
-    <row r="37" spans="1:5" ht="16.5" customHeight="1">
+    <row r="37" spans="1:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A37" s="3"/>
       <c r="C37" s="3" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
-    <row r="38" spans="1:5" ht="16.5" customHeight="1">
+    <row r="38" spans="1:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A38" s="3"/>
       <c r="C38" s="3" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
-    <row r="39" spans="1:5" ht="16.5" customHeight="1">
+    <row r="39" spans="1:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A39" s="3"/>
       <c r="C39" s="3" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
-    <row r="40" spans="1:5" ht="16.5" customHeight="1">
+    <row r="40" spans="1:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A40" s="3"/>
       <c r="C40" s="3" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
-    <row r="41" spans="1:5" ht="16.5" customHeight="1">
+    <row r="41" spans="1:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A41" s="3"/>
       <c r="C41" s="3" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
-    <row r="42" spans="1:5" ht="16.5" customHeight="1">
+    <row r="42" spans="1:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A42" s="3"/>
       <c r="C42" s="3" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
-    <row r="43" spans="1:5" ht="16.5" customHeight="1">
+    <row r="43" spans="1:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A43" s="3"/>
       <c r="C43" s="3" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
-    <row r="44" spans="1:5" ht="16.5" customHeight="1">
+    <row r="44" spans="1:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A44" s="3"/>
       <c r="C44" s="3" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
-    <row r="45" spans="1:5" ht="16.5" customHeight="1">
+    <row r="45" spans="1:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A45" s="3"/>
       <c r="C45" s="3" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
-    <row r="46" spans="1:5" ht="16.5" customHeight="1">
+    <row r="46" spans="1:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A46" s="3"/>
       <c r="C46" s="3" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
-    <row r="47" spans="1:5" ht="16.5" customHeight="1">
+    <row r="47" spans="1:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A47" s="3"/>
       <c r="C47" s="3" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
-    <row r="48" spans="1:5" ht="16.5" customHeight="1">
+    <row r="48" spans="1:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A48" s="3"/>
       <c r="C48" s="3" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
-    <row r="49" spans="1:3" ht="16.5" customHeight="1">
+    <row r="49" spans="1:3" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A49" s="3"/>
       <c r="C49" s="3" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
-    <row r="50" spans="1:3" ht="16.5" customHeight="1">
+    <row r="50" spans="1:3" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A50" s="3"/>
     </row>
-    <row r="51" spans="1:3" ht="16.5" customHeight="1">
+    <row r="51" spans="1:3" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A51" s="3"/>
     </row>
-    <row r="52" spans="1:3" ht="16.5" customHeight="1">
+    <row r="52" spans="1:3" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A52" s="3"/>
     </row>
-    <row r="53" spans="1:3" ht="16.5" customHeight="1">
+    <row r="53" spans="1:3" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A53" s="3"/>
     </row>
-    <row r="54" spans="1:3" ht="16.5" customHeight="1">
+    <row r="54" spans="1:3" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A54" s="3"/>
     </row>
-    <row r="55" spans="1:3" ht="16.5" customHeight="1">
+    <row r="55" spans="1:3" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A55" s="3"/>
     </row>
-    <row r="56" spans="1:3" ht="16.5" customHeight="1">
+    <row r="56" spans="1:3" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A56" s="3"/>
     </row>
-    <row r="57" spans="1:3" ht="16.5" customHeight="1">
+    <row r="57" spans="1:3" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A57" s="3"/>
     </row>
-    <row r="58" spans="1:3" ht="13.5">
+    <row r="58" spans="1:3" ht="13.5" x14ac:dyDescent="0.15">
       <c r="A58" s="3"/>
     </row>
-    <row r="59" spans="1:3" ht="16.5" customHeight="1">
+    <row r="59" spans="1:3" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A59" s="3"/>
     </row>
-    <row r="60" spans="1:3" ht="16.5" customHeight="1">
+    <row r="60" spans="1:3" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A60" s="3"/>
     </row>
-    <row r="61" spans="1:3" ht="16.5" customHeight="1">
+    <row r="61" spans="1:3" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A61" s="3"/>
     </row>
-    <row r="62" spans="1:3" ht="16.5" customHeight="1">
+    <row r="62" spans="1:3" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A62" s="3"/>
     </row>
-    <row r="63" spans="1:3" ht="16.5" customHeight="1">
+    <row r="63" spans="1:3" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A63" s="3"/>
     </row>
-    <row r="64" spans="1:3" ht="16.5" customHeight="1">
+    <row r="64" spans="1:3" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A64" s="3"/>
     </row>
-    <row r="65" spans="1:1" ht="16.5" customHeight="1">
+    <row r="65" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A65" s="3"/>
     </row>
-    <row r="66" spans="1:1" ht="16.5" customHeight="1">
+    <row r="66" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A66" s="3"/>
     </row>
-    <row r="67" spans="1:1" ht="16.5" customHeight="1">
+    <row r="67" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A67" s="3"/>
     </row>
-    <row r="68" spans="1:1" ht="16.5" customHeight="1">
+    <row r="68" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A68" s="3"/>
     </row>
-    <row r="69" spans="1:1" ht="16.5" customHeight="1">
+    <row r="69" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A69" s="3"/>
     </row>
-    <row r="70" spans="1:1" ht="16.5" customHeight="1">
+    <row r="70" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A70" s="3"/>
     </row>
-    <row r="71" spans="1:1" ht="16.5" customHeight="1">
+    <row r="71" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A71" s="3"/>
     </row>
-    <row r="72" spans="1:1" ht="16.5" customHeight="1">
+    <row r="72" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A72" s="3"/>
     </row>
-    <row r="73" spans="1:1" ht="16.5" customHeight="1">
+    <row r="73" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A73" s="3"/>
     </row>
-    <row r="74" spans="1:1" ht="16.5" customHeight="1">
+    <row r="74" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A74" s="3"/>
     </row>
-    <row r="75" spans="1:1" ht="16.5" customHeight="1">
+    <row r="75" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A75" s="3"/>
     </row>
-    <row r="76" spans="1:1" ht="16.5" customHeight="1">
+    <row r="76" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A76" s="3"/>
     </row>
-    <row r="77" spans="1:1" ht="16.5" customHeight="1">
+    <row r="77" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A77" s="3"/>
     </row>
-    <row r="78" spans="1:1" ht="16.5" customHeight="1">
+    <row r="78" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A78" s="3"/>
     </row>
-    <row r="79" spans="1:1" ht="16.5" customHeight="1">
+    <row r="79" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A79" s="3"/>
     </row>
-    <row r="80" spans="1:1" ht="16.5" customHeight="1">
+    <row r="80" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A80" s="3"/>
     </row>
-    <row r="81" spans="1:1" ht="16.5" customHeight="1">
+    <row r="81" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A81" s="3"/>
     </row>
-    <row r="82" spans="1:1" ht="16.5" customHeight="1">
+    <row r="82" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A82" s="3"/>
     </row>
-    <row r="83" spans="1:1" ht="16.5" customHeight="1">
+    <row r="83" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A83" s="3"/>
     </row>
-    <row r="84" spans="1:1" ht="16.5" customHeight="1">
+    <row r="84" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A84" s="3"/>
     </row>
-    <row r="85" spans="1:1" ht="16.5" customHeight="1">
+    <row r="85" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A85" s="3"/>
     </row>
-    <row r="86" spans="1:1" ht="16.5" customHeight="1">
+    <row r="86" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A86" s="3"/>
     </row>
-    <row r="87" spans="1:1" ht="16.5" customHeight="1">
+    <row r="87" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A87" s="3"/>
     </row>
-    <row r="88" spans="1:1" ht="16.5" customHeight="1">
+    <row r="88" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A88" s="3"/>
     </row>
-    <row r="89" spans="1:1" ht="16.5" customHeight="1">
+    <row r="89" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A89" s="3"/>
     </row>
-    <row r="90" spans="1:1" ht="16.5" customHeight="1">
+    <row r="90" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A90" s="3"/>
     </row>
-    <row r="91" spans="1:1" ht="16.5" customHeight="1">
+    <row r="91" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A91" s="3"/>
     </row>
-    <row r="92" spans="1:1" ht="16.5" customHeight="1">
+    <row r="92" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A92" s="3"/>
     </row>
-    <row r="93" spans="1:1" ht="16.5" customHeight="1">
+    <row r="93" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A93" s="3"/>
     </row>
-    <row r="94" spans="1:1" ht="16.5" customHeight="1">
+    <row r="94" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A94" s="3"/>
     </row>
-    <row r="95" spans="1:1" ht="16.5" customHeight="1">
+    <row r="95" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A95" s="3"/>
     </row>
-    <row r="96" spans="1:1" ht="16.5" customHeight="1">
+    <row r="96" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A96" s="3"/>
     </row>
-    <row r="97" spans="1:1" ht="16.5" customHeight="1">
+    <row r="97" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A97" s="3"/>
     </row>
-    <row r="98" spans="1:1" ht="16.5" customHeight="1">
+    <row r="98" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A98" s="3"/>
     </row>
-    <row r="99" spans="1:1" ht="16.5" customHeight="1">
+    <row r="99" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A99" s="3"/>
     </row>
-    <row r="100" spans="1:1" ht="16.5" customHeight="1">
+    <row r="100" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A100" s="3"/>
     </row>
-    <row r="101" spans="1:1" ht="16.5" customHeight="1">
+    <row r="101" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A101" s="3"/>
     </row>
-    <row r="102" spans="1:1" ht="16.5" customHeight="1">
+    <row r="102" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A102" s="3"/>
     </row>
-    <row r="103" spans="1:1" ht="16.5" customHeight="1">
+    <row r="103" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A103" s="3"/>
     </row>
-    <row r="104" spans="1:1" ht="16.5" customHeight="1">
+    <row r="104" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A104" s="3"/>
     </row>
-    <row r="105" spans="1:1" ht="16.5" customHeight="1">
+    <row r="105" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A105" s="3"/>
     </row>
-    <row r="106" spans="1:1" ht="16.5" customHeight="1">
+    <row r="106" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A106" s="3"/>
     </row>
-    <row r="107" spans="1:1" ht="16.5" customHeight="1">
+    <row r="107" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A107" s="3"/>
     </row>
-    <row r="108" spans="1:1" ht="16.5" customHeight="1">
+    <row r="108" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A108" s="3"/>
     </row>
-    <row r="109" spans="1:1" ht="16.5" customHeight="1">
+    <row r="109" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A109" s="3"/>
     </row>
-    <row r="110" spans="1:1" ht="16.5" customHeight="1">
+    <row r="110" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A110" s="3"/>
     </row>
-    <row r="111" spans="1:1" ht="16.5" customHeight="1">
+    <row r="111" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A111" s="3"/>
     </row>
-    <row r="112" spans="1:1" ht="16.5" customHeight="1">
+    <row r="112" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A112" s="3"/>
     </row>
-    <row r="113" spans="1:1" ht="16.5" customHeight="1">
+    <row r="113" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A113" s="3"/>
     </row>
-    <row r="114" spans="1:1" ht="16.5" customHeight="1">
+    <row r="114" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A114" s="3"/>
     </row>
-    <row r="115" spans="1:1" ht="16.5" customHeight="1">
+    <row r="115" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A115" s="3"/>
     </row>
-    <row r="116" spans="1:1" ht="16.5" customHeight="1">
+    <row r="116" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A116" s="3"/>
     </row>
-    <row r="117" spans="1:1" ht="16.5" customHeight="1">
+    <row r="117" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A117" s="3"/>
     </row>
-    <row r="118" spans="1:1" ht="16.5" customHeight="1">
+    <row r="118" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A118" s="3"/>
     </row>
-    <row r="119" spans="1:1" ht="16.5" customHeight="1">
+    <row r="119" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A119" s="3"/>
     </row>
-    <row r="120" spans="1:1" ht="16.5" customHeight="1">
+    <row r="120" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A120" s="3"/>
     </row>
-    <row r="121" spans="1:1" ht="16.5" customHeight="1">
+    <row r="121" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A121" s="3"/>
     </row>
-    <row r="122" spans="1:1" ht="16.5" customHeight="1">
+    <row r="122" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A122" s="3"/>
     </row>
-    <row r="123" spans="1:1" ht="16.5" customHeight="1">
+    <row r="123" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A123" s="3"/>
     </row>
-    <row r="124" spans="1:1" ht="16.5" customHeight="1">
+    <row r="124" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A124" s="3"/>
     </row>
-    <row r="125" spans="1:1" ht="16.5" customHeight="1">
+    <row r="125" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A125" s="3"/>
     </row>
-    <row r="126" spans="1:1" ht="16.5" customHeight="1">
+    <row r="126" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A126" s="3"/>
     </row>
-    <row r="127" spans="1:1" ht="16.5" customHeight="1">
+    <row r="127" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A127" s="3"/>
     </row>
-    <row r="128" spans="1:1" ht="16.5" customHeight="1">
+    <row r="128" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A128" s="3"/>
     </row>
-    <row r="129" spans="1:1" ht="16.5" customHeight="1">
+    <row r="129" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A129" s="3"/>
     </row>
-    <row r="130" spans="1:1" ht="16.5" customHeight="1">
+    <row r="130" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A130" s="3"/>
     </row>
-    <row r="131" spans="1:1" ht="16.5" customHeight="1">
+    <row r="131" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A131" s="3"/>
     </row>
-    <row r="132" spans="1:1" ht="16.5" customHeight="1">
+    <row r="132" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A132" s="3"/>
     </row>
-    <row r="133" spans="1:1" ht="16.5" customHeight="1">
+    <row r="133" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A133" s="3"/>
     </row>
-    <row r="134" spans="1:1" ht="16.5" customHeight="1">
+    <row r="134" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A134" s="3"/>
     </row>
-    <row r="135" spans="1:1" ht="16.5" customHeight="1">
+    <row r="135" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A135" s="3"/>
     </row>
-    <row r="136" spans="1:1" ht="16.5" customHeight="1">
+    <row r="136" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A136" s="3"/>
     </row>
-    <row r="137" spans="1:1" ht="16.5" customHeight="1">
+    <row r="137" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A137" s="3"/>
     </row>
-    <row r="138" spans="1:1" ht="16.5" customHeight="1">
+    <row r="138" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A138" s="3"/>
     </row>
-    <row r="139" spans="1:1" ht="16.5" customHeight="1">
+    <row r="139" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A139" s="3"/>
     </row>
-    <row r="140" spans="1:1" ht="16.5" customHeight="1">
+    <row r="140" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A140" s="3"/>
     </row>
-    <row r="141" spans="1:1" ht="16.5" customHeight="1">
+    <row r="141" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A141" s="3"/>
     </row>
-    <row r="142" spans="1:1" ht="16.5" customHeight="1">
+    <row r="142" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A142" s="3"/>
     </row>
-    <row r="143" spans="1:1" ht="16.5" customHeight="1">
+    <row r="143" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A143" s="3"/>
     </row>
-    <row r="144" spans="1:1" ht="16.5" customHeight="1">
+    <row r="144" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A144" s="3"/>
     </row>
-    <row r="145" spans="1:1" ht="16.5" customHeight="1">
+    <row r="145" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A145" s="3"/>
     </row>
-    <row r="146" spans="1:1" ht="16.5" customHeight="1">
+    <row r="146" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A146" s="3"/>
     </row>
-    <row r="147" spans="1:1" ht="16.5" customHeight="1">
+    <row r="147" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A147" s="3"/>
     </row>
-    <row r="148" spans="1:1" ht="16.5" customHeight="1">
+    <row r="148" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A148" s="3"/>
     </row>
-    <row r="149" spans="1:1" ht="16.5" customHeight="1">
+    <row r="149" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A149" s="3"/>
     </row>
-    <row r="150" spans="1:1" ht="16.5" customHeight="1">
+    <row r="150" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A150" s="3"/>
     </row>
-    <row r="151" spans="1:1" ht="16.5" customHeight="1">
+    <row r="151" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A151" s="3"/>
     </row>
-    <row r="152" spans="1:1" ht="16.5" customHeight="1">
+    <row r="152" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A152" s="3"/>
     </row>
-    <row r="153" spans="1:1" ht="16.5" customHeight="1">
+    <row r="153" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A153" s="3"/>
     </row>
-    <row r="154" spans="1:1" ht="16.5" customHeight="1">
+    <row r="154" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A154" s="3"/>
     </row>
-    <row r="155" spans="1:1" ht="16.5" customHeight="1">
+    <row r="155" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A155" s="3"/>
     </row>
-    <row r="156" spans="1:1" ht="16.5" customHeight="1">
+    <row r="156" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A156" s="3"/>
     </row>
-    <row r="157" spans="1:1" ht="16.5" customHeight="1">
+    <row r="157" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A157" s="3"/>
     </row>
-    <row r="158" spans="1:1" ht="16.5" customHeight="1">
+    <row r="158" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A158" s="3"/>
     </row>
-    <row r="159" spans="1:1" ht="16.5" customHeight="1">
+    <row r="159" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A159" s="3"/>
     </row>
-    <row r="160" spans="1:1" ht="16.5" customHeight="1">
+    <row r="160" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A160" s="3"/>
     </row>
-    <row r="161" spans="1:1" ht="16.5" customHeight="1">
+    <row r="161" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A161" s="3"/>
     </row>
-    <row r="162" spans="1:1" ht="16.5" customHeight="1">
+    <row r="162" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A162" s="3"/>
     </row>
-    <row r="163" spans="1:1" ht="16.5" customHeight="1">
+    <row r="163" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A163" s="3"/>
     </row>
-    <row r="164" spans="1:1" ht="16.5" customHeight="1">
+    <row r="164" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A164" s="3"/>
     </row>
-    <row r="165" spans="1:1" ht="16.5" customHeight="1">
+    <row r="165" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A165" s="3"/>
     </row>
-    <row r="166" spans="1:1" ht="16.5" customHeight="1">
+    <row r="166" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A166" s="3"/>
     </row>
-    <row r="167" spans="1:1" ht="16.5" customHeight="1">
+    <row r="167" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A167" s="3"/>
     </row>
   </sheetData>
-  <autoFilter ref="B1:E34"/>
+  <autoFilter ref="B1:E34" xr:uid="{00000000-0009-0000-0000-000001000000}"/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -2244,25 +2262,25 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:A14"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="55.5546875" style="1" customWidth="1"/>
     <col min="2" max="2" width="44.21875" style="1" customWidth="1"/>
     <col min="3" max="16384" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A1" s="10"/>
     </row>
-    <row r="8" spans="1:1">
+    <row r="8" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A8" s="10"/>
     </row>
-    <row r="14" spans="1:1">
+    <row r="14" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A14" s="10"/>
     </row>
   </sheetData>
@@ -2273,14 +2291,14 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:E165"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="2.77734375" style="9" customWidth="1"/>
     <col min="2" max="2" width="43.6640625" style="1" customWidth="1"/>
@@ -2290,7 +2308,7 @@
     <col min="6" max="16384" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A1" s="7"/>
       <c r="B1" s="5" t="s">
         <v>8</v>
@@ -2305,496 +2323,496 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A2" s="3"/>
     </row>
-    <row r="3" spans="1:5">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A3" s="8"/>
     </row>
-    <row r="4" spans="1:5" ht="36.75" customHeight="1">
+    <row r="4" spans="1:5" ht="36.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="3"/>
     </row>
-    <row r="5" spans="1:5">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A5" s="8"/>
     </row>
-    <row r="6" spans="1:5">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A6" s="3"/>
     </row>
-    <row r="7" spans="1:5">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A7" s="3"/>
     </row>
-    <row r="8" spans="1:5">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A8" s="3"/>
     </row>
-    <row r="9" spans="1:5">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A9" s="3"/>
     </row>
-    <row r="10" spans="1:5">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A10" s="3"/>
     </row>
-    <row r="11" spans="1:5">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A11" s="8"/>
     </row>
-    <row r="12" spans="1:5">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A12" s="3"/>
     </row>
-    <row r="13" spans="1:5">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A13" s="3"/>
     </row>
-    <row r="14" spans="1:5">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A14" s="3"/>
     </row>
-    <row r="15" spans="1:5">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A15" s="3"/>
     </row>
-    <row r="16" spans="1:5">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A16" s="3"/>
     </row>
-    <row r="17" spans="1:1">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A17" s="8"/>
     </row>
-    <row r="18" spans="1:1">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A18" s="3"/>
     </row>
-    <row r="19" spans="1:1">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A19" s="3"/>
     </row>
-    <row r="20" spans="1:1">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A20" s="3"/>
     </row>
-    <row r="21" spans="1:1">
+    <row r="21" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A21" s="3"/>
     </row>
-    <row r="22" spans="1:1">
+    <row r="22" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A22" s="3"/>
     </row>
-    <row r="23" spans="1:1">
+    <row r="23" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A23" s="8"/>
     </row>
-    <row r="24" spans="1:1">
+    <row r="24" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A24" s="3"/>
     </row>
-    <row r="25" spans="1:1">
+    <row r="25" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A25" s="3"/>
     </row>
-    <row r="26" spans="1:1">
+    <row r="26" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A26" s="3"/>
     </row>
-    <row r="27" spans="1:1">
+    <row r="27" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A27" s="3"/>
     </row>
-    <row r="28" spans="1:1">
+    <row r="28" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A28" s="3"/>
     </row>
-    <row r="29" spans="1:1">
+    <row r="29" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A29" s="8"/>
     </row>
-    <row r="30" spans="1:1">
+    <row r="30" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A30" s="8"/>
     </row>
-    <row r="31" spans="1:1">
+    <row r="31" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A31" s="3"/>
     </row>
-    <row r="32" spans="1:1">
+    <row r="32" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A32" s="3"/>
     </row>
-    <row r="33" spans="1:1">
+    <row r="33" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A33" s="3"/>
     </row>
-    <row r="34" spans="1:1">
+    <row r="34" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A34" s="3"/>
     </row>
-    <row r="35" spans="1:1">
+    <row r="35" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A35" s="8"/>
     </row>
-    <row r="36" spans="1:1">
+    <row r="36" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A36" s="8"/>
     </row>
-    <row r="37" spans="1:1">
+    <row r="37" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A37" s="8"/>
     </row>
-    <row r="38" spans="1:1">
+    <row r="38" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A38" s="8"/>
     </row>
-    <row r="39" spans="1:1">
+    <row r="39" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A39" s="8"/>
     </row>
-    <row r="40" spans="1:1">
+    <row r="40" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A40" s="8"/>
     </row>
-    <row r="41" spans="1:1">
+    <row r="41" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A41" s="8"/>
     </row>
-    <row r="42" spans="1:1">
+    <row r="42" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A42" s="8"/>
     </row>
-    <row r="43" spans="1:1">
+    <row r="43" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A43" s="8"/>
     </row>
-    <row r="44" spans="1:1">
+    <row r="44" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A44" s="8"/>
     </row>
-    <row r="45" spans="1:1">
+    <row r="45" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A45" s="8"/>
     </row>
-    <row r="46" spans="1:1">
+    <row r="46" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A46" s="8"/>
     </row>
-    <row r="47" spans="1:1">
+    <row r="47" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A47" s="8"/>
     </row>
-    <row r="48" spans="1:1">
+    <row r="48" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A48" s="8"/>
     </row>
-    <row r="49" spans="1:1">
+    <row r="49" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A49" s="8"/>
     </row>
-    <row r="50" spans="1:1">
+    <row r="50" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A50" s="8"/>
     </row>
-    <row r="51" spans="1:1">
+    <row r="51" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A51" s="8"/>
     </row>
-    <row r="52" spans="1:1">
+    <row r="52" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A52" s="8"/>
     </row>
-    <row r="53" spans="1:1">
+    <row r="53" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A53" s="8"/>
     </row>
-    <row r="54" spans="1:1">
+    <row r="54" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A54" s="8"/>
     </row>
-    <row r="55" spans="1:1">
+    <row r="55" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A55" s="8"/>
     </row>
-    <row r="56" spans="1:1">
+    <row r="56" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A56" s="8"/>
     </row>
-    <row r="57" spans="1:1">
+    <row r="57" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A57" s="8"/>
     </row>
-    <row r="58" spans="1:1">
+    <row r="58" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A58" s="8"/>
     </row>
-    <row r="59" spans="1:1">
+    <row r="59" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A59" s="8"/>
     </row>
-    <row r="60" spans="1:1">
+    <row r="60" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A60" s="8"/>
     </row>
-    <row r="61" spans="1:1">
+    <row r="61" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A61" s="8"/>
     </row>
-    <row r="62" spans="1:1">
+    <row r="62" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A62" s="8"/>
     </row>
-    <row r="63" spans="1:1">
+    <row r="63" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A63" s="8"/>
     </row>
-    <row r="64" spans="1:1">
+    <row r="64" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A64" s="8"/>
     </row>
-    <row r="65" spans="1:1">
+    <row r="65" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A65" s="8"/>
     </row>
-    <row r="66" spans="1:1">
+    <row r="66" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A66" s="8"/>
     </row>
-    <row r="67" spans="1:1">
+    <row r="67" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A67" s="8"/>
     </row>
-    <row r="68" spans="1:1">
+    <row r="68" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A68" s="8"/>
     </row>
-    <row r="69" spans="1:1">
+    <row r="69" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A69" s="8"/>
     </row>
-    <row r="70" spans="1:1">
+    <row r="70" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A70" s="8"/>
     </row>
-    <row r="71" spans="1:1">
+    <row r="71" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A71" s="8"/>
     </row>
-    <row r="72" spans="1:1">
+    <row r="72" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A72" s="8"/>
     </row>
-    <row r="73" spans="1:1">
+    <row r="73" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A73" s="8"/>
     </row>
-    <row r="74" spans="1:1">
+    <row r="74" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A74" s="8"/>
     </row>
-    <row r="75" spans="1:1">
+    <row r="75" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A75" s="8"/>
     </row>
-    <row r="76" spans="1:1">
+    <row r="76" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A76" s="8"/>
     </row>
-    <row r="77" spans="1:1">
+    <row r="77" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A77" s="8"/>
     </row>
-    <row r="78" spans="1:1">
+    <row r="78" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A78" s="8"/>
     </row>
-    <row r="79" spans="1:1">
+    <row r="79" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A79" s="8"/>
     </row>
-    <row r="80" spans="1:1">
+    <row r="80" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A80" s="8"/>
     </row>
-    <row r="81" spans="1:1">
+    <row r="81" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A81" s="8"/>
     </row>
-    <row r="82" spans="1:1">
+    <row r="82" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A82" s="8"/>
     </row>
-    <row r="83" spans="1:1">
+    <row r="83" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A83" s="8"/>
     </row>
-    <row r="84" spans="1:1">
+    <row r="84" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A84" s="8"/>
     </row>
-    <row r="85" spans="1:1">
+    <row r="85" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A85" s="8"/>
     </row>
-    <row r="86" spans="1:1">
+    <row r="86" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A86" s="8"/>
     </row>
-    <row r="87" spans="1:1">
+    <row r="87" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A87" s="8"/>
     </row>
-    <row r="88" spans="1:1">
+    <row r="88" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A88" s="8"/>
     </row>
-    <row r="89" spans="1:1">
+    <row r="89" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A89" s="8"/>
     </row>
-    <row r="90" spans="1:1">
+    <row r="90" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A90" s="8"/>
     </row>
-    <row r="91" spans="1:1">
+    <row r="91" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A91" s="8"/>
     </row>
-    <row r="92" spans="1:1">
+    <row r="92" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A92" s="8"/>
     </row>
-    <row r="93" spans="1:1">
+    <row r="93" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A93" s="8"/>
     </row>
-    <row r="94" spans="1:1">
+    <row r="94" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A94" s="8"/>
     </row>
-    <row r="95" spans="1:1">
+    <row r="95" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A95" s="8"/>
     </row>
-    <row r="96" spans="1:1">
+    <row r="96" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A96" s="8"/>
     </row>
-    <row r="97" spans="1:1">
+    <row r="97" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A97" s="8"/>
     </row>
-    <row r="98" spans="1:1">
+    <row r="98" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A98" s="8"/>
     </row>
-    <row r="99" spans="1:1">
+    <row r="99" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A99" s="8"/>
     </row>
-    <row r="100" spans="1:1">
+    <row r="100" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A100" s="8"/>
     </row>
-    <row r="101" spans="1:1">
+    <row r="101" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A101" s="8"/>
     </row>
-    <row r="102" spans="1:1">
+    <row r="102" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A102" s="8"/>
     </row>
-    <row r="103" spans="1:1">
+    <row r="103" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A103" s="8"/>
     </row>
-    <row r="104" spans="1:1">
+    <row r="104" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A104" s="8"/>
     </row>
-    <row r="105" spans="1:1">
+    <row r="105" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A105" s="8"/>
     </row>
-    <row r="106" spans="1:1">
+    <row r="106" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A106" s="8"/>
     </row>
-    <row r="107" spans="1:1">
+    <row r="107" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A107" s="8"/>
     </row>
-    <row r="108" spans="1:1">
+    <row r="108" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A108" s="8"/>
     </row>
-    <row r="109" spans="1:1">
+    <row r="109" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A109" s="8"/>
     </row>
-    <row r="110" spans="1:1">
+    <row r="110" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A110" s="8"/>
     </row>
-    <row r="111" spans="1:1">
+    <row r="111" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A111" s="8"/>
     </row>
-    <row r="112" spans="1:1">
+    <row r="112" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A112" s="8"/>
     </row>
-    <row r="113" spans="1:1">
+    <row r="113" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A113" s="8"/>
     </row>
-    <row r="114" spans="1:1">
+    <row r="114" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A114" s="8"/>
     </row>
-    <row r="115" spans="1:1">
+    <row r="115" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A115" s="8"/>
     </row>
-    <row r="116" spans="1:1">
+    <row r="116" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A116" s="8"/>
     </row>
-    <row r="117" spans="1:1">
+    <row r="117" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A117" s="8"/>
     </row>
-    <row r="118" spans="1:1">
+    <row r="118" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A118" s="8"/>
     </row>
-    <row r="119" spans="1:1">
+    <row r="119" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A119" s="8"/>
     </row>
-    <row r="120" spans="1:1">
+    <row r="120" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A120" s="8"/>
     </row>
-    <row r="121" spans="1:1">
+    <row r="121" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A121" s="8"/>
     </row>
-    <row r="122" spans="1:1">
+    <row r="122" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A122" s="8"/>
     </row>
-    <row r="123" spans="1:1">
+    <row r="123" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A123" s="8"/>
     </row>
-    <row r="124" spans="1:1">
+    <row r="124" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A124" s="8"/>
     </row>
-    <row r="125" spans="1:1">
+    <row r="125" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A125" s="8"/>
     </row>
-    <row r="126" spans="1:1">
+    <row r="126" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A126" s="8"/>
     </row>
-    <row r="127" spans="1:1">
+    <row r="127" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A127" s="8"/>
     </row>
-    <row r="128" spans="1:1">
+    <row r="128" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A128" s="8"/>
     </row>
-    <row r="129" spans="1:1">
+    <row r="129" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A129" s="8"/>
     </row>
-    <row r="130" spans="1:1">
+    <row r="130" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A130" s="8"/>
     </row>
-    <row r="131" spans="1:1">
+    <row r="131" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A131" s="8"/>
     </row>
-    <row r="132" spans="1:1">
+    <row r="132" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A132" s="8"/>
     </row>
-    <row r="133" spans="1:1">
+    <row r="133" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A133" s="8"/>
     </row>
-    <row r="134" spans="1:1">
+    <row r="134" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A134" s="8"/>
     </row>
-    <row r="135" spans="1:1">
+    <row r="135" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A135" s="8"/>
     </row>
-    <row r="136" spans="1:1">
+    <row r="136" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A136" s="8"/>
     </row>
-    <row r="137" spans="1:1">
+    <row r="137" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A137" s="8"/>
     </row>
-    <row r="138" spans="1:1">
+    <row r="138" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A138" s="8"/>
     </row>
-    <row r="139" spans="1:1">
+    <row r="139" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A139" s="8"/>
     </row>
-    <row r="140" spans="1:1">
+    <row r="140" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A140" s="8"/>
     </row>
-    <row r="141" spans="1:1">
+    <row r="141" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A141" s="8"/>
     </row>
-    <row r="142" spans="1:1">
+    <row r="142" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A142" s="8"/>
     </row>
-    <row r="143" spans="1:1">
+    <row r="143" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A143" s="8"/>
     </row>
-    <row r="144" spans="1:1">
+    <row r="144" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A144" s="8"/>
     </row>
-    <row r="145" spans="1:1">
+    <row r="145" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A145" s="8"/>
     </row>
-    <row r="146" spans="1:1">
+    <row r="146" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A146" s="8"/>
     </row>
-    <row r="147" spans="1:1">
+    <row r="147" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A147" s="8"/>
     </row>
-    <row r="148" spans="1:1">
+    <row r="148" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A148" s="8"/>
     </row>
-    <row r="149" spans="1:1">
+    <row r="149" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A149" s="8"/>
     </row>
-    <row r="150" spans="1:1">
+    <row r="150" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A150" s="8"/>
     </row>
-    <row r="151" spans="1:1">
+    <row r="151" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A151" s="8"/>
     </row>
-    <row r="152" spans="1:1">
+    <row r="152" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A152" s="8"/>
     </row>
-    <row r="153" spans="1:1">
+    <row r="153" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A153" s="8"/>
     </row>
-    <row r="154" spans="1:1">
+    <row r="154" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A154" s="8"/>
     </row>
-    <row r="155" spans="1:1">
+    <row r="155" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A155" s="8"/>
     </row>
-    <row r="156" spans="1:1">
+    <row r="156" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A156" s="8"/>
     </row>
-    <row r="157" spans="1:1">
+    <row r="157" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A157" s="8"/>
     </row>
-    <row r="158" spans="1:1">
+    <row r="158" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A158" s="8"/>
     </row>
-    <row r="159" spans="1:1">
+    <row r="159" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A159" s="8"/>
     </row>
-    <row r="160" spans="1:1">
+    <row r="160" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A160" s="8"/>
     </row>
-    <row r="161" spans="1:1">
+    <row r="161" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A161" s="8"/>
     </row>
-    <row r="162" spans="1:1">
+    <row r="162" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A162" s="8"/>
     </row>
-    <row r="163" spans="1:1">
+    <row r="163" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A163" s="8"/>
     </row>
-    <row r="164" spans="1:1">
+    <row r="164" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A164" s="8"/>
     </row>
-    <row r="165" spans="1:1">
+    <row r="165" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A165" s="8"/>
     </row>
   </sheetData>
@@ -2805,14 +2823,14 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="H36" sqref="H36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <sheetData/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Fix: no view update on item deletion
</commit_message>
<xml_diff>
--- a/docs/tasks.xlsx
+++ b/docs/tasks.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\dev\git\web\plan-it\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94790DDB-A267-45C1-BB20-6E8DB7E5C361}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E73B4EA8-D26C-492B-9AE3-7A76E08DF34E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15390" tabRatio="438" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -622,9 +622,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F165"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
@@ -767,12 +765,14 @@
       </c>
       <c r="C8" s="3" t="str">
         <f t="shared" si="0"/>
-        <v/>
+        <v>✓</v>
       </c>
       <c r="D8" s="15">
         <v>45777</v>
       </c>
-      <c r="E8" s="15"/>
+      <c r="E8" s="15">
+        <v>45834</v>
+      </c>
       <c r="F8" s="12"/>
     </row>
     <row r="9" spans="1:6" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
@@ -1441,7 +1441,7 @@
   <dimension ref="A1:F167"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -1527,10 +1527,13 @@
       </c>
       <c r="C5" s="3" t="str">
         <f t="shared" si="0"/>
-        <v/>
+        <v>✓</v>
       </c>
       <c r="D5" s="16">
         <v>45833</v>
+      </c>
+      <c r="E5" s="16">
+        <v>45834</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="33.75" customHeight="1" x14ac:dyDescent="0.15">

</xml_diff>

<commit_message>
Add dummy IPC API to interface with Electron
</commit_message>
<xml_diff>
--- a/docs/tasks.xlsx
+++ b/docs/tasks.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28925"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\dev\git\web\plan-it\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E73B4EA8-D26C-492B-9AE3-7A76E08DF34E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF96AA6F-AAFC-4845-9B92-6AE91AEE8AB0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15390" tabRatio="438" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="28">
   <si>
     <t>Task</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -147,6 +147,14 @@
   </si>
   <si>
     <t>no view update on item deletion</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>electronize</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>'created at' overwritten when modifying (regressed)</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -622,7 +630,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F165"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
@@ -811,9 +821,15 @@
     </row>
     <row r="11" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A11" s="8"/>
+      <c r="B11" s="1" t="s">
+        <v>26</v>
+      </c>
       <c r="C11" s="3" t="str">
         <f t="shared" si="0"/>
         <v/>
+      </c>
+      <c r="D11" s="16">
+        <v>45841</v>
       </c>
     </row>
     <row r="12" spans="1:6" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
@@ -1441,7 +1457,7 @@
   <dimension ref="A1:F167"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -1538,12 +1554,16 @@
     </row>
     <row r="6" spans="1:6" ht="33.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="3"/>
-      <c r="B6"/>
+      <c r="B6" s="17" t="s">
+        <v>27</v>
+      </c>
       <c r="C6" s="3" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="D6" s="15"/>
+      <c r="D6" s="15">
+        <v>45859</v>
+      </c>
       <c r="E6" s="15"/>
     </row>
     <row r="7" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">

</xml_diff>

<commit_message>
Modify Date type to string type
</commit_message>
<xml_diff>
--- a/docs/tasks.xlsx
+++ b/docs/tasks.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\dev\git\web\plan-it\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF96AA6F-AAFC-4845-9B92-6AE91AEE8AB0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8CBD3EB-2DD3-40C0-A34F-0C9FD501C681}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15390" tabRatio="438" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15390" tabRatio="438" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Requirements" sheetId="1" r:id="rId1"/>
@@ -630,9 +630,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F165"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
@@ -1456,8 +1454,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:F167"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -1552,19 +1550,21 @@
         <v>45834</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="33.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="3"/>
       <c r="B6" s="17" t="s">
         <v>27</v>
       </c>
       <c r="C6" s="3" t="str">
         <f t="shared" si="0"/>
-        <v/>
+        <v>✓</v>
       </c>
       <c r="D6" s="15">
         <v>45859</v>
       </c>
-      <c r="E6" s="15"/>
+      <c r="E6" s="15">
+        <v>45859</v>
+      </c>
     </row>
     <row r="7" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="3"/>
@@ -1585,7 +1585,7 @@
       <c r="D8" s="15"/>
       <c r="E8" s="15"/>
     </row>
-    <row r="9" spans="1:6" ht="13.5" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="3"/>
       <c r="B9"/>
       <c r="C9" s="3" t="str">
@@ -1605,14 +1605,14 @@
       <c r="D10" s="15"/>
       <c r="E10" s="15"/>
     </row>
-    <row r="11" spans="1:6" ht="36.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A11" s="3"/>
       <c r="C11" s="3" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
-    <row r="12" spans="1:6" ht="32.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A12" s="3"/>
       <c r="B12"/>
       <c r="C12" s="3" t="str">
@@ -1669,7 +1669,7 @@
         <v/>
       </c>
     </row>
-    <row r="18" spans="1:5" ht="39" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A18" s="3"/>
       <c r="B18"/>
       <c r="C18" s="3" t="str">
@@ -1679,7 +1679,7 @@
       <c r="D18" s="15"/>
       <c r="E18" s="15"/>
     </row>
-    <row r="19" spans="1:5" ht="45.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A19" s="3"/>
       <c r="B19"/>
       <c r="C19" s="3" t="str">
@@ -1709,7 +1709,7 @@
       <c r="D21" s="15"/>
       <c r="E21" s="15"/>
     </row>
-    <row r="22" spans="1:5" ht="13.5" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A22" s="3"/>
       <c r="B22"/>
       <c r="C22" s="3" t="str">
@@ -1746,7 +1746,7 @@
       <c r="D25" s="15"/>
       <c r="E25" s="15"/>
     </row>
-    <row r="26" spans="1:5" ht="34.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="26" spans="1:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A26" s="3"/>
       <c r="B26"/>
       <c r="C26" s="3" t="str">
@@ -1756,7 +1756,7 @@
       <c r="D26" s="15"/>
       <c r="E26" s="15"/>
     </row>
-    <row r="27" spans="1:5" ht="29.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="27" spans="1:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A27" s="3"/>
       <c r="B27"/>
       <c r="C27" s="3" t="str">
@@ -1783,14 +1783,14 @@
         <v/>
       </c>
     </row>
-    <row r="30" spans="1:5" ht="36.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="30" spans="1:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A30" s="3"/>
       <c r="C30" s="3" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
-    <row r="31" spans="1:5" ht="54.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="31" spans="1:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A31" s="3"/>
       <c r="B31"/>
       <c r="C31" s="3" t="str">
@@ -1830,7 +1830,7 @@
       <c r="D34" s="15"/>
       <c r="E34" s="15"/>
     </row>
-    <row r="35" spans="1:5" ht="34.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="35" spans="1:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A35" s="3"/>
       <c r="C35" s="3" t="str">
         <f t="shared" si="0"/>
@@ -1959,7 +1959,7 @@
     <row r="57" spans="1:3" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A57" s="3"/>
     </row>
-    <row r="58" spans="1:3" ht="13.5" x14ac:dyDescent="0.15">
+    <row r="58" spans="1:3" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A58" s="3"/>
     </row>
     <row r="59" spans="1:3" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">

</xml_diff>